<commit_message>
calculations and plotting fully functional
</commit_message>
<xml_diff>
--- a/SJ Fall 2022 (Oct3- Dec23) Tournaments.xlsx
+++ b/SJ Fall 2022 (Oct3- Dec23) Tournaments.xlsx
@@ -4,7 +4,7 @@
   <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet r:id="rId1" sheetId="1" name="Fall Tourneys"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="948" uniqueCount="457">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1010" uniqueCount="479">
   <si>
     <t>fullLink</t>
   </si>
@@ -1045,141 +1045,183 @@
     <t>LEVEL3</t>
   </si>
   <si>
+    <t>LEVEL2</t>
+  </si>
+  <si>
+    <t>Aryeh</t>
+  </si>
+  <si>
+    <t>A9</t>
+  </si>
+  <si>
+    <t>AnVy</t>
+  </si>
+  <si>
+    <t>AI</t>
+  </si>
+  <si>
+    <t>Boosk</t>
+  </si>
+  <si>
+    <t>Alo!</t>
+  </si>
+  <si>
+    <t>Azazel</t>
+  </si>
+  <si>
+    <t>Austi</t>
+  </si>
+  <si>
+    <t>joshathan gamer</t>
+  </si>
+  <si>
+    <t>andromeda</t>
+  </si>
+  <si>
+    <t>EO</t>
+  </si>
+  <si>
+    <t>Chocolate Jesus</t>
+  </si>
+  <si>
+    <t>justinbyleth</t>
+  </si>
+  <si>
+    <t>Chanman</t>
+  </si>
+  <si>
+    <t>Dyla</t>
+  </si>
+  <si>
+    <t>Crest</t>
+  </si>
+  <si>
+    <t>marcus</t>
+  </si>
+  <si>
+    <t>Charm</t>
+  </si>
+  <si>
+    <t>HunterWinthorpe</t>
+  </si>
+  <si>
+    <t>Grey</t>
+  </si>
+  <si>
+    <t>mateo</t>
+  </si>
+  <si>
+    <t>Cipher</t>
+  </si>
+  <si>
+    <t>Kurama</t>
+  </si>
+  <si>
+    <t>Sly</t>
+  </si>
+  <si>
+    <t>mega</t>
+  </si>
+  <si>
+    <t>Consent is Badass</t>
+  </si>
+  <si>
+    <t>WheeZy</t>
+  </si>
+  <si>
+    <t>Secret</t>
+  </si>
+  <si>
+    <t>Noodl</t>
+  </si>
+  <si>
+    <t>Critz</t>
+  </si>
+  <si>
+    <t>Jacie</t>
+  </si>
+  <si>
+    <t>SoulheartRS</t>
+  </si>
+  <si>
+    <t>pharaoh</t>
+  </si>
+  <si>
+    <t>freege</t>
+  </si>
+  <si>
+    <t>Blase</t>
+  </si>
+  <si>
+    <t>Spectro</t>
+  </si>
+  <si>
+    <t>ranger</t>
+  </si>
+  <si>
+    <t>Hoodinii</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>Yeast</t>
+  </si>
+  <si>
+    <t>Snogi</t>
+  </si>
+  <si>
+    <t>Sauce</t>
+  </si>
+  <si>
+    <t>Zeusie</t>
+  </si>
+  <si>
     <t>Spiro</t>
   </si>
   <si>
-    <t>Hoodinii</t>
-  </si>
-  <si>
-    <t>Jacie</t>
-  </si>
-  <si>
-    <t>Noodl</t>
-  </si>
-  <si>
-    <t>Sauce</t>
-  </si>
-  <si>
-    <t>WheeZy</t>
-  </si>
-  <si>
-    <t>Aryeh</t>
+    <t>seabass</t>
+  </si>
+  <si>
+    <t>Vince</t>
+  </si>
+  <si>
+    <t>skies</t>
+  </si>
+  <si>
+    <t>Yoshi-o</t>
+  </si>
+  <si>
+    <t>Treestain</t>
+  </si>
+  <si>
+    <t>haze</t>
   </si>
   <si>
     <t>Xavier</t>
   </si>
   <si>
-    <t>EO</t>
-  </si>
-  <si>
-    <t>Vince</t>
-  </si>
-  <si>
-    <t>A9</t>
-  </si>
-  <si>
-    <t>HunterWinthorpe</t>
-  </si>
-  <si>
-    <t>AKFirez</t>
-  </si>
-  <si>
-    <t>Treestain</t>
-  </si>
-  <si>
-    <t>Kurama</t>
-  </si>
-  <si>
-    <t>Boosk</t>
-  </si>
-  <si>
-    <t>Charm</t>
-  </si>
-  <si>
-    <t>Alo!</t>
-  </si>
-  <si>
-    <t>Snogi</t>
-  </si>
-  <si>
-    <t>Dyla</t>
-  </si>
-  <si>
-    <t>AnVy</t>
-  </si>
-  <si>
     <t>critz but retired</t>
   </si>
   <si>
-    <t>Chanman</t>
-  </si>
-  <si>
-    <t>Critz</t>
+    <t>Poop87</t>
   </si>
   <si>
     <t>&lt;3 brisket</t>
   </si>
   <si>
-    <t>Poop87</t>
-  </si>
-  <si>
-    <t>Azazel</t>
-  </si>
-  <si>
-    <t>yoshi-o</t>
-  </si>
-  <si>
-    <t>Consent is Badass</t>
-  </si>
-  <si>
-    <t>ranger</t>
-  </si>
-  <si>
-    <t>Cipher</t>
-  </si>
-  <si>
-    <t>pharaoh</t>
-  </si>
-  <si>
-    <t>skies</t>
-  </si>
-  <si>
-    <t>mega</t>
-  </si>
-  <si>
     <t>chan</t>
   </si>
   <si>
-    <t>mateo</t>
-  </si>
-  <si>
-    <t>andromeda</t>
-  </si>
-  <si>
-    <t>joshathan gamer</t>
-  </si>
-  <si>
-    <t>haze</t>
-  </si>
-  <si>
-    <t>marcus</t>
-  </si>
-  <si>
-    <t>seabass</t>
-  </si>
-  <si>
-    <t>justinbyleth</t>
-  </si>
-  <si>
-    <t>freege</t>
+    <t>xavier</t>
+  </si>
+  <si>
+    <t>hotsaucefuego</t>
   </si>
   <si>
     <t>obmcbob</t>
   </si>
   <si>
-    <t>hotsaucefuego</t>
-  </si>
-  <si>
     <t>Hyperlink</t>
   </si>
   <si>
@@ -1340,6 +1382,30 @@
   </si>
   <si>
     <t>critz but retired~~~1$$Vince~~~2$$Noodl~~~3$$Hoodinii~~~4$$AnVy~~~5$$Treestain~~~5$$Blase~~~7$$WheeZy~~~7$$zeusie~~~9$$Dyla~~~9$$Grey~~~9$$Sauce~~~9$$AUSTI~~~13$$HunterWinthorpe~~~13$$xavier~~~13$$Secret~~~13$$PoP~~~17$$Steezus~~~17$$ModernYasha~~~17$$feelingkettle~~~17$$Oppan Ganon Style~~~17$$ThePsychicBoy~~~17$$kino.~~~17$$DizzY~~~17$$Joba~~~25$$Steve~~~25$$</t>
+  </si>
+  <si>
+    <t>https://www.start.gg/tournament/hyperspace-ultimate-24/details</t>
+  </si>
+  <si>
+    <t>hyperspace-ultimate-24</t>
+  </si>
+  <si>
+    <t>Hyperspace Ultimate 24</t>
+  </si>
+  <si>
+    <t>EO~~~1$$Menchu~~~2$$$Krilldog$~~~3$$ShyTy~~~4$$ccoma~~~5$$B2THICK~~~5$$Shigga_Sears~~~7$$Chocolate Jesus~~~7$$ZBosGaming~~~9$$Yeast~~~9$$Venture~~~9$$</t>
+  </si>
+  <si>
+    <t>https://www.start.gg/tournament/battle-over-the-bridge-68/events</t>
+  </si>
+  <si>
+    <t>battle-over-the-bridge-68</t>
+  </si>
+  <si>
+    <t>Battle Over The Bridge 68</t>
+  </si>
+  <si>
+    <t>xavier~~~1$$Alo!~~~2$$Aryeh~~~3$$Blase~~~4$$WheeZy~~~5$$Dyla~~~5$$Secret~~~7$$Benitez~~~7$$feelingkettle~~~9$$Hurricane~~~9$$Ham Burrito~~~9$$The Real Mr. M~~~9$$ToasterGaming22~~~13$$ThePsychicBoy~~~13$$</t>
   </si>
   <si>
     <t>Pbj Holiday Palooza</t>
@@ -1395,7 +1461,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1417,6 +1483,12 @@
       <family val="2"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1428,6 +1500,12 @@
       <sz val="11"/>
       <color rgb="FF1155cc"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
@@ -1528,7 +1606,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="30">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1546,7 +1624,7 @@
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general" wrapText="1"/>
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
@@ -1560,43 +1638,61 @@
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="4" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="5" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="4" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="6" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="4" applyFont="1" fillId="5" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="7" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="4" applyFont="1" fillId="6" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="8" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="4" applyFont="1" fillId="7" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="9" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="4" applyFont="1" fillId="8" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="4" applyFont="1" fillId="9" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general" wrapText="1"/>
-    </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="6" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="7" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="8" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1907,263 +2003,263 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="11" width="15.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="11" width="15.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="11" width="19.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="15" width="15.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="15" width="15.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="15" width="19.576428571428572" customWidth="1" bestFit="1"/>
     <col min="4" max="4" style="6" width="16.005" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="11" width="16.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="11" width="16.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="11" width="20.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="11" width="18.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="15" width="16.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="15" width="16.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="15" width="20.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="14" width="18.719285714285714" customWidth="1" bestFit="1"/>
     <col min="9" max="9" style="6" width="31.14785714285714" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="30">
-      <c r="A1" s="12" t="s">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="30" customFormat="1" s="1">
+      <c r="A1" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="C1" s="14" t="s">
-        <v>443</v>
-      </c>
-      <c r="D1" s="15" t="s">
+      <c r="C1" s="20" t="s">
+        <v>465</v>
+      </c>
+      <c r="D1" s="21" t="s">
         <v>159</v>
       </c>
-      <c r="E1" s="16" t="s">
-        <v>444</v>
-      </c>
-      <c r="F1" s="17" t="s">
+      <c r="E1" s="22" t="s">
+        <v>466</v>
+      </c>
+      <c r="F1" s="23" t="s">
         <v>289</v>
       </c>
-      <c r="G1" s="18" t="s">
-        <v>445</v>
-      </c>
-      <c r="H1" s="10"/>
-      <c r="I1" s="19" t="s">
-        <v>446</v>
+      <c r="G1" s="24" t="s">
+        <v>467</v>
+      </c>
+      <c r="H1" s="16"/>
+      <c r="I1" s="25" t="s">
+        <v>468</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="66" customFormat="1" s="1">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="26" t="s">
         <v>50</v>
       </c>
-      <c r="C2" s="20" t="s">
+      <c r="C2" s="26" t="s">
         <v>133</v>
       </c>
-      <c r="D2" s="20" t="s">
+      <c r="D2" s="26" t="s">
         <v>156</v>
       </c>
-      <c r="E2" s="20" t="s">
+      <c r="E2" s="26" t="s">
         <v>228</v>
       </c>
-      <c r="F2" s="20" t="s">
+      <c r="F2" s="26" t="s">
         <v>286</v>
       </c>
-      <c r="G2" s="20" t="s">
+      <c r="G2" s="26" t="s">
         <v>323</v>
       </c>
-      <c r="H2" s="21"/>
-      <c r="I2" s="20" t="s">
-        <v>447</v>
+      <c r="H2" s="27"/>
+      <c r="I2" s="26" t="s">
+        <v>469</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="66" customFormat="1" s="1">
-      <c r="A3" s="20" t="s">
+      <c r="A3" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="20" t="s">
+      <c r="B3" s="26" t="s">
         <v>59</v>
       </c>
-      <c r="C3" s="20" t="s">
+      <c r="C3" s="26" t="s">
         <v>142</v>
       </c>
-      <c r="D3" s="20" t="s">
+      <c r="D3" s="26" t="s">
         <v>165</v>
       </c>
-      <c r="E3" s="20" t="s">
+      <c r="E3" s="26" t="s">
         <v>237</v>
       </c>
-      <c r="F3" s="20" t="s">
+      <c r="F3" s="26" t="s">
         <v>295</v>
       </c>
-      <c r="G3" s="20" t="s">
+      <c r="G3" s="26" t="s">
         <v>332</v>
       </c>
-      <c r="H3" s="21"/>
-      <c r="I3" s="20" t="s">
-        <v>448</v>
+      <c r="H3" s="27"/>
+      <c r="I3" s="26" t="s">
+        <v>470</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="66" customFormat="1" s="1">
-      <c r="A4" s="20" t="s">
+      <c r="A4" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="B4" s="20" t="s">
+      <c r="B4" s="26" t="s">
         <v>66</v>
       </c>
-      <c r="C4" s="20" t="s">
+      <c r="C4" s="26" t="s">
         <v>149</v>
       </c>
-      <c r="D4" s="20" t="s">
+      <c r="D4" s="26" t="s">
         <v>172</v>
       </c>
-      <c r="E4" s="20" t="s">
+      <c r="E4" s="26" t="s">
         <v>244</v>
       </c>
-      <c r="F4" s="20" t="s">
+      <c r="F4" s="26" t="s">
         <v>302</v>
       </c>
       <c r="G4" s="2"/>
-      <c r="H4" s="21"/>
-      <c r="I4" s="20" t="s">
-        <v>449</v>
+      <c r="H4" s="27"/>
+      <c r="I4" s="26" t="s">
+        <v>471</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="75.75">
       <c r="A5" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B5" s="20" t="s">
+      <c r="B5" s="26" t="s">
         <v>73</v>
       </c>
       <c r="C5" s="2"/>
-      <c r="D5" s="20" t="s">
+      <c r="D5" s="26" t="s">
         <v>179</v>
       </c>
-      <c r="E5" s="20" t="s">
+      <c r="E5" s="26" t="s">
         <v>251</v>
       </c>
-      <c r="F5" s="20" t="s">
+      <c r="F5" s="26" t="s">
         <v>309</v>
       </c>
       <c r="G5" s="2"/>
       <c r="H5" s="8" t="s">
-        <v>450</v>
-      </c>
-      <c r="I5" s="20" t="s">
-        <v>451</v>
+        <v>472</v>
+      </c>
+      <c r="I5" s="26" t="s">
+        <v>473</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="66" customFormat="1" s="1">
-      <c r="A6" s="22" t="s">
+      <c r="A6" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="B6" s="20" t="s">
+      <c r="B6" s="26" t="s">
         <v>80</v>
       </c>
       <c r="C6" s="2"/>
-      <c r="D6" s="20" t="s">
+      <c r="D6" s="26" t="s">
         <v>186</v>
       </c>
-      <c r="E6" s="20" t="s">
+      <c r="E6" s="26" t="s">
         <v>258</v>
       </c>
-      <c r="F6" s="20" t="s">
+      <c r="F6" s="26" t="s">
         <v>316</v>
       </c>
       <c r="G6" s="2"/>
-      <c r="H6" s="21"/>
-      <c r="I6" s="23" t="s">
-        <v>452</v>
+      <c r="H6" s="27"/>
+      <c r="I6" s="29" t="s">
+        <v>474</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="78" customFormat="1" s="1">
       <c r="A7" s="2"/>
-      <c r="B7" s="20" t="s">
+      <c r="B7" s="26" t="s">
         <v>86</v>
       </c>
       <c r="C7" s="2"/>
-      <c r="D7" s="20" t="s">
+      <c r="D7" s="26" t="s">
         <v>193</v>
       </c>
-      <c r="E7" s="20" t="s">
+      <c r="E7" s="26" t="s">
         <v>265</v>
       </c>
-      <c r="F7" s="21"/>
+      <c r="F7" s="27"/>
       <c r="G7" s="2"/>
-      <c r="H7" s="21"/>
-      <c r="I7" s="23" t="s">
-        <v>453</v>
+      <c r="H7" s="27"/>
+      <c r="I7" s="29" t="s">
+        <v>475</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="66" customFormat="1" s="1">
       <c r="A8" s="2"/>
-      <c r="B8" s="20" t="s">
+      <c r="B8" s="26" t="s">
         <v>93</v>
       </c>
       <c r="C8" s="2"/>
-      <c r="D8" s="20" t="s">
+      <c r="D8" s="26" t="s">
         <v>200</v>
       </c>
-      <c r="E8" s="20" t="s">
+      <c r="E8" s="26" t="s">
         <v>272</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
-      <c r="H8" s="21"/>
-      <c r="I8" s="23" t="s">
-        <v>454</v>
+      <c r="H8" s="27"/>
+      <c r="I8" s="29" t="s">
+        <v>476</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="66" customFormat="1" s="1">
       <c r="A9" s="2"/>
-      <c r="B9" s="20" t="s">
+      <c r="B9" s="26" t="s">
         <v>99</v>
       </c>
       <c r="C9" s="2"/>
-      <c r="D9" s="20" t="s">
+      <c r="D9" s="26" t="s">
         <v>207</v>
       </c>
-      <c r="E9" s="20" t="s">
+      <c r="E9" s="26" t="s">
         <v>279</v>
       </c>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
-      <c r="H9" s="21"/>
-      <c r="I9" s="20" t="s">
-        <v>455</v>
+      <c r="H9" s="27"/>
+      <c r="I9" s="26" t="s">
+        <v>477</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="66" customFormat="1" s="1">
       <c r="A10" s="2"/>
-      <c r="B10" s="20" t="s">
+      <c r="B10" s="26" t="s">
         <v>106</v>
       </c>
       <c r="C10" s="2"/>
-      <c r="D10" s="20" t="s">
+      <c r="D10" s="26" t="s">
         <v>214</v>
       </c>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
-      <c r="H10" s="21"/>
-      <c r="I10" s="20" t="s">
-        <v>456</v>
+      <c r="H10" s="27"/>
+      <c r="I10" s="26" t="s">
+        <v>478</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="66" customFormat="1" s="1">
       <c r="A11" s="2"/>
-      <c r="B11" s="20" t="s">
+      <c r="B11" s="26" t="s">
         <v>113</v>
       </c>
       <c r="C11" s="2"/>
-      <c r="D11" s="20" t="s">
+      <c r="D11" s="26" t="s">
         <v>221</v>
       </c>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
-      <c r="H11" s="21"/>
-      <c r="I11" s="21"/>
+      <c r="H11" s="27"/>
+      <c r="I11" s="27"/>
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5" customFormat="1" s="1">
       <c r="A12" s="2"/>
-      <c r="B12" s="20" t="s">
+      <c r="B12" s="26" t="s">
         <v>120</v>
       </c>
       <c r="C12" s="2"/>
@@ -2171,12 +2267,12 @@
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
-      <c r="H12" s="21"/>
-      <c r="I12" s="21"/>
+      <c r="H12" s="27"/>
+      <c r="I12" s="27"/>
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5" customFormat="1" s="1">
       <c r="A13" s="2"/>
-      <c r="B13" s="20" t="s">
+      <c r="B13" s="26" t="s">
         <v>126</v>
       </c>
       <c r="C13" s="2"/>
@@ -2184,19 +2280,19 @@
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
-      <c r="H13" s="21"/>
-      <c r="I13" s="21"/>
+      <c r="H13" s="27"/>
+      <c r="I13" s="27"/>
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
       <c r="A14" s="8"/>
       <c r="B14" s="8"/>
       <c r="C14" s="8"/>
-      <c r="D14" s="21"/>
+      <c r="D14" s="27"/>
       <c r="E14" s="8"/>
       <c r="F14" s="8"/>
       <c r="G14" s="8"/>
       <c r="H14" s="10"/>
-      <c r="I14" s="21"/>
+      <c r="I14" s="27"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2208,9 +2304,9 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:N46"/>
+  <dimension ref="A1:N48"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2220,7 +2316,7 @@
     <col min="4" max="4" style="6" width="16.433571428571426" customWidth="1" bestFit="1"/>
     <col min="5" max="5" style="6" width="14.147857142857141" customWidth="1" bestFit="1"/>
     <col min="6" max="6" style="7" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="6" width="43.86214285714286" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="6" width="25.14785714285714" customWidth="1" bestFit="1"/>
     <col min="8" max="8" style="6" width="43.86214285714286" customWidth="1" bestFit="1"/>
     <col min="9" max="9" style="6" width="43.86214285714286" customWidth="1" bestFit="1"/>
     <col min="10" max="10" style="6" width="43.86214285714286" customWidth="1" bestFit="1"/>
@@ -2230,18 +2326,18 @@
     <col min="14" max="14" style="7" width="43.86214285714286" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="38.25" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="32.25" customFormat="1" s="1">
       <c r="A1" s="2" t="s">
-        <v>387</v>
+        <v>401</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>388</v>
+        <v>402</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>389</v>
+        <v>403</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>390</v>
+        <v>404</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>4</v>
@@ -2250,7 +2346,7 @@
         <v>5</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>391</v>
+        <v>405</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>7</v>
@@ -2271,10 +2367,10 @@
         <v>12</v>
       </c>
       <c r="N1" s="3" t="s">
-        <v>392</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5" customFormat="1" s="1">
+        <v>406</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="138" customFormat="1" s="1">
       <c r="A2" s="4" t="s">
         <v>13</v>
       </c>
@@ -2294,7 +2390,7 @@
         <v>21</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>393</v>
+        <v>407</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>306</v>
@@ -2303,7 +2399,7 @@
         <v>306</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>394</v>
+        <v>408</v>
       </c>
       <c r="K2" s="5">
         <v>0</v>
@@ -2318,7 +2414,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="85.5" customFormat="1" s="1">
       <c r="A3" s="4" t="s">
         <v>22</v>
       </c>
@@ -2338,7 +2434,7 @@
         <v>13</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>395</v>
+        <v>409</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>306</v>
@@ -2347,7 +2443,7 @@
         <v>306</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>394</v>
+        <v>408</v>
       </c>
       <c r="K3" s="5">
         <v>0</v>
@@ -2362,7 +2458,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="58.5" customFormat="1" s="1">
       <c r="A4" s="4" t="s">
         <v>29</v>
       </c>
@@ -2382,7 +2478,7 @@
         <v>8</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>396</v>
+        <v>410</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>306</v>
@@ -2391,7 +2487,7 @@
         <v>306</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>394</v>
+        <v>408</v>
       </c>
       <c r="K4" s="5">
         <v>0</v>
@@ -2406,7 +2502,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="48.75" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="47.25" customFormat="1" s="1">
       <c r="A5" s="4" t="s">
         <v>36</v>
       </c>
@@ -2414,7 +2510,7 @@
         <v>37</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>397</v>
+        <v>411</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>16</v>
@@ -2426,7 +2522,7 @@
         <v>7</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>398</v>
+        <v>412</v>
       </c>
       <c r="H5" s="2" t="s">
         <v>306</v>
@@ -2435,7 +2531,7 @@
         <v>306</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>394</v>
+        <v>408</v>
       </c>
       <c r="K5" s="5">
         <v>0</v>
@@ -2450,7 +2546,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="61.5" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="124.5" customFormat="1" s="1">
       <c r="A6" s="4" t="s">
         <v>43</v>
       </c>
@@ -2458,7 +2554,7 @@
         <v>44</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>399</v>
+        <v>413</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>16</v>
@@ -2470,7 +2566,7 @@
         <v>20</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>400</v>
+        <v>414</v>
       </c>
       <c r="H6" s="2" t="s">
         <v>306</v>
@@ -2479,7 +2575,7 @@
         <v>306</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>394</v>
+        <v>408</v>
       </c>
       <c r="K6" s="5">
         <v>0</v>
@@ -2494,7 +2590,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="58.5" customFormat="1" s="1">
       <c r="A7" s="4" t="s">
         <v>50</v>
       </c>
@@ -2514,7 +2610,7 @@
         <v>10</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>401</v>
+        <v>415</v>
       </c>
       <c r="H7" s="2" t="s">
         <v>306</v>
@@ -2523,7 +2619,7 @@
         <v>306</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>394</v>
+        <v>408</v>
       </c>
       <c r="K7" s="5">
         <v>0</v>
@@ -2538,7 +2634,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="72" customFormat="1" s="1">
       <c r="A8" s="4" t="s">
         <v>59</v>
       </c>
@@ -2558,7 +2654,7 @@
         <v>9</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>402</v>
+        <v>416</v>
       </c>
       <c r="H8" s="2" t="s">
         <v>306</v>
@@ -2567,7 +2663,7 @@
         <v>306</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>394</v>
+        <v>408</v>
       </c>
       <c r="K8" s="5">
         <v>0</v>
@@ -2582,7 +2678,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="47.25" customFormat="1" s="1">
       <c r="A9" s="4" t="s">
         <v>66</v>
       </c>
@@ -2602,7 +2698,7 @@
         <v>6</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>403</v>
+        <v>417</v>
       </c>
       <c r="H9" s="2" t="s">
         <v>306</v>
@@ -2611,7 +2707,7 @@
         <v>306</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>394</v>
+        <v>408</v>
       </c>
       <c r="K9" s="5">
         <v>0</v>
@@ -2626,7 +2722,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="58.5" customFormat="1" s="1">
       <c r="A10" s="4" t="s">
         <v>73</v>
       </c>
@@ -2646,7 +2742,7 @@
         <v>11</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>404</v>
+        <v>418</v>
       </c>
       <c r="H10" s="2" t="s">
         <v>306</v>
@@ -2655,7 +2751,7 @@
         <v>306</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>394</v>
+        <v>408</v>
       </c>
       <c r="K10" s="5">
         <v>0</v>
@@ -2670,7 +2766,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="72" customFormat="1" s="1">
       <c r="A11" s="4" t="s">
         <v>80</v>
       </c>
@@ -2690,7 +2786,7 @@
         <v>9</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>405</v>
+        <v>419</v>
       </c>
       <c r="H11" s="2" t="s">
         <v>306</v>
@@ -2699,7 +2795,7 @@
         <v>306</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>394</v>
+        <v>408</v>
       </c>
       <c r="K11" s="5">
         <v>0</v>
@@ -2734,7 +2830,7 @@
         <v>21</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>406</v>
+        <v>420</v>
       </c>
       <c r="H12" s="2" t="s">
         <v>306</v>
@@ -2743,7 +2839,7 @@
         <v>306</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>394</v>
+        <v>408</v>
       </c>
       <c r="K12" s="5">
         <v>0</v>
@@ -2778,7 +2874,7 @@
         <v>10</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>407</v>
+        <v>421</v>
       </c>
       <c r="H13" s="2" t="s">
         <v>306</v>
@@ -2787,7 +2883,7 @@
         <v>306</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>394</v>
+        <v>408</v>
       </c>
       <c r="K13" s="5">
         <v>0</v>
@@ -2822,16 +2918,16 @@
         <v>8</v>
       </c>
       <c r="G14" s="2" t="s">
+        <v>422</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="J14" s="2" t="s">
         <v>408</v>
-      </c>
-      <c r="H14" s="2" t="s">
-        <v>306</v>
-      </c>
-      <c r="I14" s="2" t="s">
-        <v>306</v>
-      </c>
-      <c r="J14" s="2" t="s">
-        <v>394</v>
       </c>
       <c r="K14" s="5">
         <v>0</v>
@@ -2866,7 +2962,7 @@
         <v>7</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>409</v>
+        <v>423</v>
       </c>
       <c r="H15" s="2" t="s">
         <v>306</v>
@@ -2875,7 +2971,7 @@
         <v>306</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>394</v>
+        <v>408</v>
       </c>
       <c r="K15" s="5">
         <v>0</v>
@@ -2910,7 +3006,7 @@
         <v>8</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>410</v>
+        <v>424</v>
       </c>
       <c r="H16" s="2" t="s">
         <v>306</v>
@@ -2919,7 +3015,7 @@
         <v>306</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>394</v>
+        <v>408</v>
       </c>
       <c r="K16" s="5">
         <v>0</v>
@@ -2954,7 +3050,7 @@
         <v>12</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>411</v>
+        <v>425</v>
       </c>
       <c r="H17" s="2" t="s">
         <v>306</v>
@@ -2963,7 +3059,7 @@
         <v>306</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>394</v>
+        <v>408</v>
       </c>
       <c r="K17" s="5">
         <v>0</v>
@@ -2998,7 +3094,7 @@
         <v>20</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>412</v>
+        <v>426</v>
       </c>
       <c r="H18" s="2" t="s">
         <v>306</v>
@@ -3007,7 +3103,7 @@
         <v>306</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>394</v>
+        <v>408</v>
       </c>
       <c r="K18" s="5">
         <v>0</v>
@@ -3042,7 +3138,7 @@
         <v>27</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>413</v>
+        <v>427</v>
       </c>
       <c r="H19" s="2" t="s">
         <v>306</v>
@@ -3051,7 +3147,7 @@
         <v>306</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>394</v>
+        <v>408</v>
       </c>
       <c r="K19" s="5">
         <v>0</v>
@@ -3086,7 +3182,7 @@
         <v>21</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>414</v>
+        <v>428</v>
       </c>
       <c r="H20" s="2" t="s">
         <v>306</v>
@@ -3095,7 +3191,7 @@
         <v>306</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>394</v>
+        <v>408</v>
       </c>
       <c r="K20" s="5">
         <v>0</v>
@@ -3130,7 +3226,7 @@
         <v>32</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>415</v>
+        <v>429</v>
       </c>
       <c r="H21" s="2" t="s">
         <v>306</v>
@@ -3139,7 +3235,7 @@
         <v>306</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>394</v>
+        <v>408</v>
       </c>
       <c r="K21" s="5">
         <v>0</v>
@@ -3174,7 +3270,7 @@
         <v>14</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>416</v>
+        <v>430</v>
       </c>
       <c r="H22" s="2" t="s">
         <v>306</v>
@@ -3183,7 +3279,7 @@
         <v>306</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>394</v>
+        <v>408</v>
       </c>
       <c r="K22" s="5">
         <v>0</v>
@@ -3218,7 +3314,7 @@
         <v>12</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>417</v>
+        <v>431</v>
       </c>
       <c r="H23" s="2" t="s">
         <v>306</v>
@@ -3227,7 +3323,7 @@
         <v>306</v>
       </c>
       <c r="J23" s="2" t="s">
-        <v>394</v>
+        <v>408</v>
       </c>
       <c r="K23" s="5">
         <v>0</v>
@@ -3262,7 +3358,7 @@
         <v>18</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>418</v>
+        <v>432</v>
       </c>
       <c r="H24" s="2" t="s">
         <v>306</v>
@@ -3271,7 +3367,7 @@
         <v>306</v>
       </c>
       <c r="J24" s="2" t="s">
-        <v>394</v>
+        <v>408</v>
       </c>
       <c r="K24" s="5">
         <v>0</v>
@@ -3306,7 +3402,7 @@
         <v>19</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>419</v>
+        <v>433</v>
       </c>
       <c r="H25" s="2" t="s">
         <v>306</v>
@@ -3315,7 +3411,7 @@
         <v>306</v>
       </c>
       <c r="J25" s="2" t="s">
-        <v>394</v>
+        <v>408</v>
       </c>
       <c r="K25" s="5">
         <v>0</v>
@@ -3350,7 +3446,7 @@
         <v>15</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>420</v>
+        <v>434</v>
       </c>
       <c r="H26" s="2" t="s">
         <v>306</v>
@@ -3359,7 +3455,7 @@
         <v>306</v>
       </c>
       <c r="J26" s="2" t="s">
-        <v>394</v>
+        <v>408</v>
       </c>
       <c r="K26" s="5">
         <v>0</v>
@@ -3394,7 +3490,7 @@
         <v>16</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>421</v>
+        <v>435</v>
       </c>
       <c r="H27" s="2" t="s">
         <v>306</v>
@@ -3403,7 +3499,7 @@
         <v>306</v>
       </c>
       <c r="J27" s="2" t="s">
-        <v>394</v>
+        <v>408</v>
       </c>
       <c r="K27" s="5">
         <v>0</v>
@@ -3438,7 +3534,7 @@
         <v>14</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>422</v>
+        <v>436</v>
       </c>
       <c r="H28" s="2" t="s">
         <v>306</v>
@@ -3447,7 +3543,7 @@
         <v>306</v>
       </c>
       <c r="J28" s="2" t="s">
-        <v>394</v>
+        <v>408</v>
       </c>
       <c r="K28" s="5">
         <v>0</v>
@@ -3482,7 +3578,7 @@
         <v>16</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>423</v>
+        <v>437</v>
       </c>
       <c r="H29" s="2" t="s">
         <v>306</v>
@@ -3491,7 +3587,7 @@
         <v>306</v>
       </c>
       <c r="J29" s="2" t="s">
-        <v>394</v>
+        <v>408</v>
       </c>
       <c r="K29" s="5">
         <v>0</v>
@@ -3526,7 +3622,7 @@
         <v>13</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>424</v>
+        <v>438</v>
       </c>
       <c r="H30" s="2" t="s">
         <v>306</v>
@@ -3535,7 +3631,7 @@
         <v>306</v>
       </c>
       <c r="J30" s="2" t="s">
-        <v>394</v>
+        <v>408</v>
       </c>
       <c r="K30" s="5">
         <v>0</v>
@@ -3570,7 +3666,7 @@
         <v>16</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>425</v>
+        <v>439</v>
       </c>
       <c r="H31" s="2" t="s">
         <v>306</v>
@@ -3579,7 +3675,7 @@
         <v>306</v>
       </c>
       <c r="J31" s="2" t="s">
-        <v>394</v>
+        <v>408</v>
       </c>
       <c r="K31" s="5">
         <v>0</v>
@@ -3614,7 +3710,7 @@
         <v>39</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>426</v>
+        <v>440</v>
       </c>
       <c r="H32" s="2" t="s">
         <v>306</v>
@@ -3623,7 +3719,7 @@
         <v>306</v>
       </c>
       <c r="J32" s="2" t="s">
-        <v>394</v>
+        <v>408</v>
       </c>
       <c r="K32" s="5">
         <v>0</v>
@@ -3658,7 +3754,7 @@
         <v>40</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>427</v>
+        <v>441</v>
       </c>
       <c r="H33" s="2" t="s">
         <v>306</v>
@@ -3667,7 +3763,7 @@
         <v>306</v>
       </c>
       <c r="J33" s="2" t="s">
-        <v>394</v>
+        <v>408</v>
       </c>
       <c r="K33" s="5">
         <v>0</v>
@@ -3702,7 +3798,7 @@
         <v>21</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>428</v>
+        <v>442</v>
       </c>
       <c r="H34" s="2" t="s">
         <v>306</v>
@@ -3711,7 +3807,7 @@
         <v>306</v>
       </c>
       <c r="J34" s="2" t="s">
-        <v>394</v>
+        <v>408</v>
       </c>
       <c r="K34" s="5">
         <v>0</v>
@@ -3746,7 +3842,7 @@
         <v>31</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>429</v>
+        <v>443</v>
       </c>
       <c r="H35" s="2" t="s">
         <v>306</v>
@@ -3755,7 +3851,7 @@
         <v>306</v>
       </c>
       <c r="J35" s="2" t="s">
-        <v>394</v>
+        <v>408</v>
       </c>
       <c r="K35" s="5">
         <v>0</v>
@@ -3790,7 +3886,7 @@
         <v>30</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>430</v>
+        <v>444</v>
       </c>
       <c r="H36" s="2" t="s">
         <v>306</v>
@@ -3799,7 +3895,7 @@
         <v>306</v>
       </c>
       <c r="J36" s="2" t="s">
-        <v>394</v>
+        <v>408</v>
       </c>
       <c r="K36" s="5">
         <v>0</v>
@@ -3834,7 +3930,7 @@
         <v>33</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>431</v>
+        <v>445</v>
       </c>
       <c r="H37" s="2" t="s">
         <v>306</v>
@@ -3843,7 +3939,7 @@
         <v>306</v>
       </c>
       <c r="J37" s="2" t="s">
-        <v>394</v>
+        <v>408</v>
       </c>
       <c r="K37" s="5">
         <v>0</v>
@@ -3878,7 +3974,7 @@
         <v>26</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>432</v>
+        <v>446</v>
       </c>
       <c r="H38" s="2" t="s">
         <v>306</v>
@@ -3887,7 +3983,7 @@
         <v>306</v>
       </c>
       <c r="J38" s="2" t="s">
-        <v>394</v>
+        <v>408</v>
       </c>
       <c r="K38" s="5">
         <v>0</v>
@@ -3922,7 +4018,7 @@
         <v>32</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>433</v>
+        <v>447</v>
       </c>
       <c r="H39" s="2" t="s">
         <v>306</v>
@@ -3931,7 +4027,7 @@
         <v>306</v>
       </c>
       <c r="J39" s="2" t="s">
-        <v>394</v>
+        <v>408</v>
       </c>
       <c r="K39" s="5">
         <v>0</v>
@@ -3966,7 +4062,7 @@
         <v>13</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>434</v>
+        <v>448</v>
       </c>
       <c r="H40" s="2" t="s">
         <v>306</v>
@@ -3975,7 +4071,7 @@
         <v>306</v>
       </c>
       <c r="J40" s="2" t="s">
-        <v>394</v>
+        <v>408</v>
       </c>
       <c r="K40" s="5">
         <v>0</v>
@@ -4010,7 +4106,7 @@
         <v>10</v>
       </c>
       <c r="G41" s="2" t="s">
-        <v>435</v>
+        <v>449</v>
       </c>
       <c r="H41" s="2" t="s">
         <v>306</v>
@@ -4019,7 +4115,7 @@
         <v>306</v>
       </c>
       <c r="J41" s="2" t="s">
-        <v>394</v>
+        <v>408</v>
       </c>
       <c r="K41" s="5">
         <v>0</v>
@@ -4054,7 +4150,7 @@
         <v>6</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>436</v>
+        <v>450</v>
       </c>
       <c r="H42" s="2" t="s">
         <v>306</v>
@@ -4063,7 +4159,7 @@
         <v>306</v>
       </c>
       <c r="J42" s="2" t="s">
-        <v>394</v>
+        <v>408</v>
       </c>
       <c r="K42" s="5">
         <v>0</v>
@@ -4098,7 +4194,7 @@
         <v>13</v>
       </c>
       <c r="G43" s="2" t="s">
-        <v>437</v>
+        <v>451</v>
       </c>
       <c r="H43" s="2" t="s">
         <v>306</v>
@@ -4107,7 +4203,7 @@
         <v>306</v>
       </c>
       <c r="J43" s="2" t="s">
-        <v>394</v>
+        <v>408</v>
       </c>
       <c r="K43" s="5">
         <v>0</v>
@@ -4142,7 +4238,7 @@
         <v>14</v>
       </c>
       <c r="G44" s="2" t="s">
-        <v>438</v>
+        <v>452</v>
       </c>
       <c r="H44" s="2" t="s">
         <v>306</v>
@@ -4151,7 +4247,7 @@
         <v>306</v>
       </c>
       <c r="J44" s="2" t="s">
-        <v>394</v>
+        <v>408</v>
       </c>
       <c r="K44" s="5">
         <v>0</v>
@@ -4174,7 +4270,7 @@
         <v>324</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>439</v>
+        <v>453</v>
       </c>
       <c r="D45" s="2" t="s">
         <v>326</v>
@@ -4186,7 +4282,7 @@
         <v>26</v>
       </c>
       <c r="G45" s="2" t="s">
-        <v>440</v>
+        <v>454</v>
       </c>
       <c r="H45" s="2" t="s">
         <v>306</v>
@@ -4195,7 +4291,7 @@
         <v>306</v>
       </c>
       <c r="J45" s="2" t="s">
-        <v>394</v>
+        <v>408</v>
       </c>
       <c r="K45" s="5">
         <v>0</v>
@@ -4211,46 +4307,134 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="19.5" customFormat="1" s="1">
-      <c r="A46" s="4" t="s">
+      <c r="A46" s="16" t="s">
+        <v>455</v>
+      </c>
+      <c r="B46" s="16" t="s">
+        <v>456</v>
+      </c>
+      <c r="C46" s="16" t="s">
+        <v>457</v>
+      </c>
+      <c r="D46" s="16" t="s">
+        <v>326</v>
+      </c>
+      <c r="E46" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="F46" s="17">
+        <v>11</v>
+      </c>
+      <c r="G46" s="16" t="s">
+        <v>458</v>
+      </c>
+      <c r="H46" s="16" t="s">
+        <v>306</v>
+      </c>
+      <c r="I46" s="16" t="s">
+        <v>306</v>
+      </c>
+      <c r="J46" s="16" t="s">
+        <v>408</v>
+      </c>
+      <c r="K46" s="17">
+        <v>0</v>
+      </c>
+      <c r="L46" s="17">
+        <v>0</v>
+      </c>
+      <c r="M46" s="17">
+        <v>0</v>
+      </c>
+      <c r="N46" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="19.5" customFormat="1" s="1">
+      <c r="A47" s="16" t="s">
+        <v>459</v>
+      </c>
+      <c r="B47" s="16" t="s">
+        <v>460</v>
+      </c>
+      <c r="C47" s="16" t="s">
+        <v>461</v>
+      </c>
+      <c r="D47" s="16" t="s">
+        <v>326</v>
+      </c>
+      <c r="E47" s="16" t="s">
+        <v>160</v>
+      </c>
+      <c r="F47" s="17">
+        <v>14</v>
+      </c>
+      <c r="G47" s="16" t="s">
+        <v>462</v>
+      </c>
+      <c r="H47" s="16" t="s">
+        <v>306</v>
+      </c>
+      <c r="I47" s="16" t="s">
+        <v>306</v>
+      </c>
+      <c r="J47" s="16" t="s">
+        <v>408</v>
+      </c>
+      <c r="K47" s="17">
+        <v>0</v>
+      </c>
+      <c r="L47" s="17">
+        <v>0</v>
+      </c>
+      <c r="M47" s="17">
+        <v>0</v>
+      </c>
+      <c r="N47" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="19.5" customFormat="1" s="1">
+      <c r="A48" s="4" t="s">
         <v>332</v>
       </c>
-      <c r="B46" s="2" t="s">
+      <c r="B48" s="2" t="s">
         <v>333</v>
       </c>
-      <c r="C46" s="2" t="s">
-        <v>441</v>
-      </c>
-      <c r="D46" s="2" t="s">
+      <c r="C48" s="2" t="s">
+        <v>463</v>
+      </c>
+      <c r="D48" s="2" t="s">
         <v>326</v>
       </c>
-      <c r="E46" s="2" t="s">
+      <c r="E48" s="2" t="s">
         <v>327</v>
       </c>
-      <c r="F46" s="5">
+      <c r="F48" s="5">
         <v>43</v>
       </c>
-      <c r="G46" s="2" t="s">
-        <v>442</v>
-      </c>
-      <c r="H46" s="2" t="s">
-        <v>306</v>
-      </c>
-      <c r="I46" s="2" t="s">
-        <v>306</v>
-      </c>
-      <c r="J46" s="2" t="s">
-        <v>394</v>
-      </c>
-      <c r="K46" s="5">
-        <v>0</v>
-      </c>
-      <c r="L46" s="5">
-        <v>0</v>
-      </c>
-      <c r="M46" s="5">
-        <v>0</v>
-      </c>
-      <c r="N46" s="5">
+      <c r="G48" s="2" t="s">
+        <v>464</v>
+      </c>
+      <c r="H48" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="I48" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="J48" s="2" t="s">
+        <v>408</v>
+      </c>
+      <c r="K48" s="5">
+        <v>0</v>
+      </c>
+      <c r="L48" s="5">
+        <v>0</v>
+      </c>
+      <c r="M48" s="5">
+        <v>0</v>
+      </c>
+      <c r="N48" s="5">
         <v>0</v>
       </c>
     </row>
@@ -4264,15 +4448,16 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="11" width="14.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="11" width="15.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="11" width="15.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="14" width="14.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="15" width="15.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="14" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="14" width="15.43357142857143" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
@@ -4285,191 +4470,335 @@
       <c r="C1" s="8" t="s">
         <v>341</v>
       </c>
+      <c r="D1" s="8" t="s">
+        <v>342</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
       <c r="A2" s="8" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>344</v>
+        <v>345</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>346</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
       <c r="A3" s="8" t="s">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>346</v>
+        <v>348</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>347</v>
+        <v>349</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>350</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
       <c r="A4" s="8" t="s">
-        <v>348</v>
+        <v>351</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>350</v>
+        <v>353</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>354</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
       <c r="A5" s="8" t="s">
-        <v>351</v>
+        <v>355</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>352</v>
+        <v>356</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+        <v>357</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
       <c r="A6" s="8" t="s">
-        <v>354</v>
+        <v>359</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>355</v>
+        <v>360</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+        <v>361</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
       <c r="A7" s="8" t="s">
-        <v>357</v>
+        <v>363</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>358</v>
+        <v>364</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
+        <v>365</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
       <c r="A8" s="8" t="s">
-        <v>360</v>
+        <v>367</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>361</v>
+        <v>368</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
-      <c r="A9" s="8" t="s">
-        <v>363</v>
+        <v>369</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
+      <c r="A9" s="9" t="s">
+        <v>371</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>364</v>
+        <v>372</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
-      <c r="A10" s="8" t="s">
-        <v>366</v>
+        <v>373</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
+      <c r="A10" s="10" t="s">
+        <v>375</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>367</v>
+        <v>376</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
-      <c r="A11" s="8" t="s">
-        <v>369</v>
+        <v>377</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
+      <c r="A11" s="10" t="s">
+        <v>379</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>370</v>
-      </c>
-      <c r="C11" s="8"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
+        <v>380</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>381</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
       <c r="A12" s="8" t="s">
-        <v>371</v>
+        <v>383</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>372</v>
-      </c>
-      <c r="C12" s="8"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
-      <c r="A13" s="8" t="s">
-        <v>373</v>
+        <v>384</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>381</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
+      <c r="A13" s="10" t="s">
+        <v>386</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>374</v>
-      </c>
-      <c r="C13" s="8"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
-      <c r="A14" s="8" t="s">
-        <v>375</v>
+        <v>387</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>381</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
+      <c r="A14" s="10" t="s">
+        <v>388</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>376</v>
-      </c>
-      <c r="C14" s="8"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
-      <c r="A15" s="8" t="s">
-        <v>377</v>
+        <v>389</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>381</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
+      <c r="A15" s="10" t="s">
+        <v>390</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>378</v>
-      </c>
-      <c r="C15" s="8"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
-      <c r="A16" s="8" t="s">
-        <v>379</v>
+        <v>391</v>
+      </c>
+      <c r="C15" s="11" t="s">
+        <v>381</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
+      <c r="A16" s="10" t="s">
+        <v>392</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>380</v>
-      </c>
-      <c r="C16" s="8"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
-      <c r="A17" s="8" t="s">
+        <v>393</v>
+      </c>
+      <c r="C16" s="11" t="s">
         <v>381</v>
       </c>
-      <c r="B17" s="8" t="s">
-        <v>382</v>
-      </c>
-      <c r="C17" s="8"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
-      <c r="A18" s="9" t="s">
-        <v>383</v>
+      <c r="D16" s="11" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
+      <c r="A17" s="11" t="s">
+        <v>381</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>381</v>
+      </c>
+      <c r="C17" s="10"/>
+      <c r="D17" s="11" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
+      <c r="A18" s="8" t="s">
+        <v>394</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>384</v>
-      </c>
-      <c r="C18" s="8"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
-      <c r="A19" s="10"/>
+        <v>395</v>
+      </c>
+      <c r="C18" s="10"/>
+      <c r="D18" s="11" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5">
+      <c r="A19" s="8" t="s">
+        <v>396</v>
+      </c>
       <c r="B19" s="8" t="s">
-        <v>385</v>
+        <v>397</v>
       </c>
       <c r="C19" s="10"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
-      <c r="A20" s="10"/>
+      <c r="D19" s="12" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5">
+      <c r="A20" s="12" t="s">
+        <v>381</v>
+      </c>
       <c r="B20" s="8" t="s">
-        <v>386</v>
+        <v>398</v>
       </c>
       <c r="C20" s="10"/>
+      <c r="D20" s="12" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="19.5">
+      <c r="A21" s="11" t="s">
+        <v>381</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>399</v>
+      </c>
+      <c r="C21" s="10"/>
+      <c r="D21" s="12" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="19.5">
+      <c r="A22" s="11" t="s">
+        <v>381</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>400</v>
+      </c>
+      <c r="C22" s="10"/>
+      <c r="D22" s="12" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="19.5">
+      <c r="A23" s="11" t="s">
+        <v>381</v>
+      </c>
+      <c r="B23" s="11" t="s">
+        <v>381</v>
+      </c>
+      <c r="C23" s="10"/>
+      <c r="D23" s="12" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="19.5">
+      <c r="A24" s="12" t="s">
+        <v>381</v>
+      </c>
+      <c r="B24" s="11" t="s">
+        <v>381</v>
+      </c>
+      <c r="C24" s="10"/>
+      <c r="D24" s="12" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="19.5">
+      <c r="A25" s="10"/>
+      <c r="B25" s="13" t="s">
+        <v>381</v>
+      </c>
+      <c r="C25" s="10"/>
+      <c r="D25" s="10"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75">
+      <c r="A26" s="12" t="s">
+        <v>381</v>
+      </c>
+      <c r="B26" s="11" t="s">
+        <v>381</v>
+      </c>
+      <c r="C26" s="10"/>
+      <c r="D26" s="12" t="s">
+        <v>381</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4488,8 +4817,8 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="6" width="40.71928571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="6" width="41.86214285714286" customWidth="1" bestFit="1"/>
     <col min="4" max="4" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="5" max="5" style="6" width="6.2907142857142855" customWidth="1" bestFit="1"/>
     <col min="6" max="6" style="7" width="8.576428571428572" customWidth="1" bestFit="1"/>

</xml_diff>

<commit_message>
should have committed sooner but here is current best alg calcs i have
</commit_message>
<xml_diff>
--- a/SJ Fall 2022 (Oct3- Dec23) Tournaments.xlsx
+++ b/SJ Fall 2022 (Oct3- Dec23) Tournaments.xlsx
@@ -10,14 +10,14 @@
     <sheet r:id="rId1" sheetId="1" name="Fall Tourneys"/>
     <sheet r:id="rId2" sheetId="2" name="Results Sheet Test"/>
     <sheet r:id="rId3" sheetId="3" name="Player Info Test"/>
-    <sheet r:id="rId4" sheetId="4" name="Tourney Result OUTPUT"/>
+    <sheet r:id="rId4" sheetId="4" name="TODO not used"/>
   </sheets>
   <calcPr fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1010" uniqueCount="479">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="990" uniqueCount="482">
   <si>
     <t>fullLink</t>
   </si>
@@ -1162,9 +1162,6 @@
     <t>Hoodinii</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t>Yeast</t>
   </si>
   <si>
@@ -1183,12 +1180,18 @@
     <t>seabass</t>
   </si>
   <si>
+    <t>Cougy</t>
+  </si>
+  <si>
     <t>Vince</t>
   </si>
   <si>
     <t>skies</t>
   </si>
   <si>
+    <t>LS</t>
+  </si>
+  <si>
     <t>Yoshi-o</t>
   </si>
   <si>
@@ -1408,19 +1411,25 @@
     <t>xavier~~~1$$Alo!~~~2$$Aryeh~~~3$$Blase~~~4$$WheeZy~~~5$$Dyla~~~5$$Secret~~~7$$Benitez~~~7$$feelingkettle~~~9$$Hurricane~~~9$$Ham Burrito~~~9$$The Real Mr. M~~~9$$ToasterGaming22~~~13$$ThePsychicBoy~~~13$$</t>
   </si>
   <si>
+    <t>https://www.start.gg/tournament/smash-ultimate-at-south-jersey-geek-fest-2022-fall/events</t>
+  </si>
+  <si>
+    <t>smash-ultimate-at-south-jersey-geek-fest-2022-fall</t>
+  </si>
+  <si>
+    <t>SJ Geek Fest</t>
+  </si>
+  <si>
+    <t>Other Tourneys</t>
+  </si>
+  <si>
+    <t>Aryeh~~~1$$Ls~~~2$$Xavier~~~3$$EO~~~4$$feelingkettle~~~5$$WheeZy~~~5$$SuperYoshi141~~~7$$VINN~~~7$$Vailskibum94~~~9$$Yoshiya Zeper~~~9$$Unown~~~9$$Grey~~~9$$Crimson Ninja~~~13$$Ian~~~13$$MCheese~~~13$$Unown69~~~13$$Yikes~~~17$$</t>
+  </si>
+  <si>
     <t>Pbj Holiday Palooza</t>
   </si>
   <si>
     <t>Yoshi-O~~~1$$Mateo~~~2$$Noodl~~~3$$Ranger~~~4$$Haze~~~5$$Marcus~~~5$$critz but retired~~~7$$AnVy~~~7$$Charm~~~9$$Aryeh~~~9$$Critz~~~9$$Hoodinii~~~9$$Blase~~~13$$A9~~~13$$xavier~~~13$$Sauce~~~13$$Woanpul~~~17$$flackito~~~17$$Kyruya~~~17$$AUSTI~~~17$$Crest~~~17$$HunterWinthorpe~~~17$$Spectro~~~17$$Kurama~~~17$$sethis~~~25$$Orochi~~~25$$PoP~~~25$$.gpg~~~25$$Visada~~~25$$$Krilldog$~~~25$$feelingkettle~~~25$$WheeZy~~~25$$ThePsychicBoy~~~33$$Blackmoon~~~33$$koala cub~~~33$$kino.~~~33$$Vailskibum94~~~33$$Keg~~~33$$Joba~~~33$$Steezus~~~33$$AlexAWG~~~33$$Spidey 99~~~33$$Dyla~~~33$$</t>
-  </si>
-  <si>
-    <t>Pop the Bubble / PBJ</t>
-  </si>
-  <si>
-    <t>Rowan</t>
-  </si>
-  <si>
-    <t>Other Tourneys</t>
   </si>
   <si>
     <t>September Tourneys not for Fall PR</t>
@@ -1489,6 +1498,12 @@
       <family val="2"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1500,12 +1515,6 @@
       <sz val="11"/>
       <color rgb="FF1155cc"/>
       <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
@@ -1606,7 +1615,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="29">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1638,13 +1647,7 @@
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" quotePrefix="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -1653,34 +1656,37 @@
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="4" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="4" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="5" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="4" applyFont="1" fillId="5" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="5" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="4" applyFont="1" fillId="6" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="5" applyFont="1" fillId="5" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="4" applyFont="1" fillId="7" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="5" applyFont="1" fillId="6" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="4" applyFont="1" fillId="8" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="5" applyFont="1" fillId="7" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="4" applyFont="1" fillId="9" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="5" applyFont="1" fillId="8" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="5" applyFont="1" fillId="9" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
@@ -2003,18 +2009,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="15" width="15.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="15" width="15.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="15" width="19.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="13" width="15.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="13" width="15.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="13" width="19.576428571428572" customWidth="1" bestFit="1"/>
     <col min="4" max="4" style="6" width="16.005" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="15" width="16.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="15" width="16.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="15" width="20.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="14" width="18.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="13" width="16.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="13" width="16.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="13" width="20.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="12" width="18.719285714285714" customWidth="1" bestFit="1"/>
     <col min="9" max="9" style="6" width="31.14785714285714" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="30" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="32.25" customFormat="1" s="1">
       <c r="A1" s="18" t="s">
         <v>16</v>
       </c>
@@ -2022,13 +2028,13 @@
         <v>53</v>
       </c>
       <c r="C1" s="20" t="s">
-        <v>465</v>
+        <v>136</v>
       </c>
       <c r="D1" s="21" t="s">
         <v>159</v>
       </c>
       <c r="E1" s="22" t="s">
-        <v>466</v>
+        <v>231</v>
       </c>
       <c r="F1" s="23" t="s">
         <v>289</v>
@@ -2036,12 +2042,12 @@
       <c r="G1" s="24" t="s">
         <v>467</v>
       </c>
-      <c r="H1" s="16"/>
+      <c r="H1" s="14"/>
       <c r="I1" s="25" t="s">
-        <v>468</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="66" customFormat="1" s="1">
+        <v>471</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="72" customFormat="1" s="1">
       <c r="A2" s="26" t="s">
         <v>13</v>
       </c>
@@ -2063,12 +2069,12 @@
       <c r="G2" s="26" t="s">
         <v>323</v>
       </c>
-      <c r="H2" s="27"/>
+      <c r="H2" s="14"/>
       <c r="I2" s="26" t="s">
-        <v>469</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="66" customFormat="1" s="1">
+        <v>472</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="85.5" customFormat="1" s="1">
       <c r="A3" s="26" t="s">
         <v>22</v>
       </c>
@@ -2090,12 +2096,12 @@
       <c r="G3" s="26" t="s">
         <v>332</v>
       </c>
-      <c r="H3" s="27"/>
+      <c r="H3" s="14"/>
       <c r="I3" s="26" t="s">
-        <v>470</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="66" customFormat="1" s="1">
+        <v>473</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="72" customFormat="1" s="1">
       <c r="A4" s="26" t="s">
         <v>29</v>
       </c>
@@ -2115,12 +2121,12 @@
         <v>302</v>
       </c>
       <c r="G4" s="2"/>
-      <c r="H4" s="27"/>
+      <c r="H4" s="14"/>
       <c r="I4" s="26" t="s">
-        <v>471</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="75.75">
+        <v>474</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="72">
       <c r="A5" s="4" t="s">
         <v>36</v>
       </c>
@@ -2139,14 +2145,14 @@
       </c>
       <c r="G5" s="2"/>
       <c r="H5" s="8" t="s">
-        <v>472</v>
+        <v>475</v>
       </c>
       <c r="I5" s="26" t="s">
-        <v>473</v>
+        <v>476</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="66" customFormat="1" s="1">
-      <c r="A6" s="28" t="s">
+      <c r="A6" s="27" t="s">
         <v>43</v>
       </c>
       <c r="B6" s="26" t="s">
@@ -2163,9 +2169,9 @@
         <v>316</v>
       </c>
       <c r="G6" s="2"/>
-      <c r="H6" s="27"/>
-      <c r="I6" s="29" t="s">
-        <v>474</v>
+      <c r="H6" s="14"/>
+      <c r="I6" s="28" t="s">
+        <v>477</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="78" customFormat="1" s="1">
@@ -2180,11 +2186,11 @@
       <c r="E7" s="26" t="s">
         <v>265</v>
       </c>
-      <c r="F7" s="27"/>
+      <c r="F7" s="14"/>
       <c r="G7" s="2"/>
-      <c r="H7" s="27"/>
-      <c r="I7" s="29" t="s">
-        <v>475</v>
+      <c r="H7" s="14"/>
+      <c r="I7" s="28" t="s">
+        <v>478</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="66" customFormat="1" s="1">
@@ -2201,9 +2207,9 @@
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
-      <c r="H8" s="27"/>
-      <c r="I8" s="29" t="s">
-        <v>476</v>
+      <c r="H8" s="14"/>
+      <c r="I8" s="28" t="s">
+        <v>479</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="66" customFormat="1" s="1">
@@ -2220,9 +2226,9 @@
       </c>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
-      <c r="H9" s="27"/>
+      <c r="H9" s="14"/>
       <c r="I9" s="26" t="s">
-        <v>477</v>
+        <v>480</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="66" customFormat="1" s="1">
@@ -2237,9 +2243,9 @@
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
-      <c r="H10" s="27"/>
+      <c r="H10" s="14"/>
       <c r="I10" s="26" t="s">
-        <v>478</v>
+        <v>481</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="66" customFormat="1" s="1">
@@ -2254,8 +2260,8 @@
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
-      <c r="H11" s="27"/>
-      <c r="I11" s="27"/>
+      <c r="H11" s="14"/>
+      <c r="I11" s="14"/>
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5" customFormat="1" s="1">
       <c r="A12" s="2"/>
@@ -2267,8 +2273,8 @@
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
-      <c r="H12" s="27"/>
-      <c r="I12" s="27"/>
+      <c r="H12" s="14"/>
+      <c r="I12" s="14"/>
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5" customFormat="1" s="1">
       <c r="A13" s="2"/>
@@ -2280,19 +2286,19 @@
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
-      <c r="H13" s="27"/>
-      <c r="I13" s="27"/>
+      <c r="H13" s="14"/>
+      <c r="I13" s="14"/>
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
       <c r="A14" s="8"/>
       <c r="B14" s="8"/>
       <c r="C14" s="8"/>
-      <c r="D14" s="27"/>
+      <c r="D14" s="14"/>
       <c r="E14" s="8"/>
       <c r="F14" s="8"/>
       <c r="G14" s="8"/>
       <c r="H14" s="10"/>
-      <c r="I14" s="27"/>
+      <c r="I14" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2304,7 +2310,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:N48"/>
+  <dimension ref="A1:N49"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2328,16 +2334,16 @@
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="32.25" customFormat="1" s="1">
       <c r="A1" s="2" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>4</v>
@@ -2346,7 +2352,7 @@
         <v>5</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>7</v>
@@ -2367,7 +2373,7 @@
         <v>12</v>
       </c>
       <c r="N1" s="3" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="138" customFormat="1" s="1">
@@ -2390,7 +2396,7 @@
         <v>21</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>306</v>
@@ -2399,7 +2405,7 @@
         <v>306</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="K2" s="5">
         <v>0</v>
@@ -2434,16 +2440,16 @@
         <v>13</v>
       </c>
       <c r="G3" s="2" t="s">
+        <v>410</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="J3" s="2" t="s">
         <v>409</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>306</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>306</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>408</v>
       </c>
       <c r="K3" s="5">
         <v>0</v>
@@ -2478,7 +2484,7 @@
         <v>8</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>306</v>
@@ -2487,7 +2493,7 @@
         <v>306</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="K4" s="5">
         <v>0</v>
@@ -2510,7 +2516,7 @@
         <v>37</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>16</v>
@@ -2522,7 +2528,7 @@
         <v>7</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="H5" s="2" t="s">
         <v>306</v>
@@ -2531,7 +2537,7 @@
         <v>306</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="K5" s="5">
         <v>0</v>
@@ -2554,7 +2560,7 @@
         <v>44</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>16</v>
@@ -2566,7 +2572,7 @@
         <v>20</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="H6" s="2" t="s">
         <v>306</v>
@@ -2575,7 +2581,7 @@
         <v>306</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="K6" s="5">
         <v>0</v>
@@ -2610,7 +2616,7 @@
         <v>10</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="H7" s="2" t="s">
         <v>306</v>
@@ -2619,7 +2625,7 @@
         <v>306</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="K7" s="5">
         <v>0</v>
@@ -2654,7 +2660,7 @@
         <v>9</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="H8" s="2" t="s">
         <v>306</v>
@@ -2663,7 +2669,7 @@
         <v>306</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="K8" s="5">
         <v>0</v>
@@ -2698,7 +2704,7 @@
         <v>6</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="H9" s="2" t="s">
         <v>306</v>
@@ -2707,7 +2713,7 @@
         <v>306</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="K9" s="5">
         <v>0</v>
@@ -2742,7 +2748,7 @@
         <v>11</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="H10" s="2" t="s">
         <v>306</v>
@@ -2751,7 +2757,7 @@
         <v>306</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="K10" s="5">
         <v>0</v>
@@ -2786,7 +2792,7 @@
         <v>9</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="H11" s="2" t="s">
         <v>306</v>
@@ -2795,7 +2801,7 @@
         <v>306</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="K11" s="5">
         <v>0</v>
@@ -2830,7 +2836,7 @@
         <v>21</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="H12" s="2" t="s">
         <v>306</v>
@@ -2839,7 +2845,7 @@
         <v>306</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="K12" s="5">
         <v>0</v>
@@ -2874,7 +2880,7 @@
         <v>10</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="H13" s="2" t="s">
         <v>306</v>
@@ -2883,7 +2889,7 @@
         <v>306</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="K13" s="5">
         <v>0</v>
@@ -2918,7 +2924,7 @@
         <v>8</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="H14" s="2" t="s">
         <v>306</v>
@@ -2927,7 +2933,7 @@
         <v>306</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="K14" s="5">
         <v>0</v>
@@ -2962,7 +2968,7 @@
         <v>7</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="H15" s="2" t="s">
         <v>306</v>
@@ -2971,7 +2977,7 @@
         <v>306</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="K15" s="5">
         <v>0</v>
@@ -3006,7 +3012,7 @@
         <v>8</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="H16" s="2" t="s">
         <v>306</v>
@@ -3015,7 +3021,7 @@
         <v>306</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="K16" s="5">
         <v>0</v>
@@ -3050,7 +3056,7 @@
         <v>12</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="H17" s="2" t="s">
         <v>306</v>
@@ -3059,7 +3065,7 @@
         <v>306</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="K17" s="5">
         <v>0</v>
@@ -3094,7 +3100,7 @@
         <v>20</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="H18" s="2" t="s">
         <v>306</v>
@@ -3103,7 +3109,7 @@
         <v>306</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="K18" s="5">
         <v>0</v>
@@ -3138,7 +3144,7 @@
         <v>27</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="H19" s="2" t="s">
         <v>306</v>
@@ -3147,7 +3153,7 @@
         <v>306</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="K19" s="5">
         <v>0</v>
@@ -3182,7 +3188,7 @@
         <v>21</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="H20" s="2" t="s">
         <v>306</v>
@@ -3191,7 +3197,7 @@
         <v>306</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="K20" s="5">
         <v>0</v>
@@ -3226,7 +3232,7 @@
         <v>32</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="H21" s="2" t="s">
         <v>306</v>
@@ -3235,7 +3241,7 @@
         <v>306</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="K21" s="5">
         <v>0</v>
@@ -3270,7 +3276,7 @@
         <v>14</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="H22" s="2" t="s">
         <v>306</v>
@@ -3279,7 +3285,7 @@
         <v>306</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="K22" s="5">
         <v>0</v>
@@ -3314,7 +3320,7 @@
         <v>12</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="H23" s="2" t="s">
         <v>306</v>
@@ -3323,7 +3329,7 @@
         <v>306</v>
       </c>
       <c r="J23" s="2" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="K23" s="5">
         <v>0</v>
@@ -3358,7 +3364,7 @@
         <v>18</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="H24" s="2" t="s">
         <v>306</v>
@@ -3367,7 +3373,7 @@
         <v>306</v>
       </c>
       <c r="J24" s="2" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="K24" s="5">
         <v>0</v>
@@ -3402,7 +3408,7 @@
         <v>19</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="H25" s="2" t="s">
         <v>306</v>
@@ -3411,7 +3417,7 @@
         <v>306</v>
       </c>
       <c r="J25" s="2" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="K25" s="5">
         <v>0</v>
@@ -3446,7 +3452,7 @@
         <v>15</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="H26" s="2" t="s">
         <v>306</v>
@@ -3455,7 +3461,7 @@
         <v>306</v>
       </c>
       <c r="J26" s="2" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="K26" s="5">
         <v>0</v>
@@ -3490,7 +3496,7 @@
         <v>16</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="H27" s="2" t="s">
         <v>306</v>
@@ -3499,7 +3505,7 @@
         <v>306</v>
       </c>
       <c r="J27" s="2" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="K27" s="5">
         <v>0</v>
@@ -3534,7 +3540,7 @@
         <v>14</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="H28" s="2" t="s">
         <v>306</v>
@@ -3543,7 +3549,7 @@
         <v>306</v>
       </c>
       <c r="J28" s="2" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="K28" s="5">
         <v>0</v>
@@ -3578,7 +3584,7 @@
         <v>16</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="H29" s="2" t="s">
         <v>306</v>
@@ -3587,7 +3593,7 @@
         <v>306</v>
       </c>
       <c r="J29" s="2" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="K29" s="5">
         <v>0</v>
@@ -3622,7 +3628,7 @@
         <v>13</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="H30" s="2" t="s">
         <v>306</v>
@@ -3631,7 +3637,7 @@
         <v>306</v>
       </c>
       <c r="J30" s="2" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="K30" s="5">
         <v>0</v>
@@ -3666,7 +3672,7 @@
         <v>16</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="H31" s="2" t="s">
         <v>306</v>
@@ -3675,7 +3681,7 @@
         <v>306</v>
       </c>
       <c r="J31" s="2" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="K31" s="5">
         <v>0</v>
@@ -3710,7 +3716,7 @@
         <v>39</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="H32" s="2" t="s">
         <v>306</v>
@@ -3719,7 +3725,7 @@
         <v>306</v>
       </c>
       <c r="J32" s="2" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="K32" s="5">
         <v>0</v>
@@ -3754,7 +3760,7 @@
         <v>40</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="H33" s="2" t="s">
         <v>306</v>
@@ -3763,7 +3769,7 @@
         <v>306</v>
       </c>
       <c r="J33" s="2" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="K33" s="5">
         <v>0</v>
@@ -3798,7 +3804,7 @@
         <v>21</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="H34" s="2" t="s">
         <v>306</v>
@@ -3807,7 +3813,7 @@
         <v>306</v>
       </c>
       <c r="J34" s="2" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="K34" s="5">
         <v>0</v>
@@ -3842,7 +3848,7 @@
         <v>31</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="H35" s="2" t="s">
         <v>306</v>
@@ -3851,7 +3857,7 @@
         <v>306</v>
       </c>
       <c r="J35" s="2" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="K35" s="5">
         <v>0</v>
@@ -3886,7 +3892,7 @@
         <v>30</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="H36" s="2" t="s">
         <v>306</v>
@@ -3895,7 +3901,7 @@
         <v>306</v>
       </c>
       <c r="J36" s="2" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="K36" s="5">
         <v>0</v>
@@ -3930,7 +3936,7 @@
         <v>33</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="H37" s="2" t="s">
         <v>306</v>
@@ -3939,7 +3945,7 @@
         <v>306</v>
       </c>
       <c r="J37" s="2" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="K37" s="5">
         <v>0</v>
@@ -3974,7 +3980,7 @@
         <v>26</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="H38" s="2" t="s">
         <v>306</v>
@@ -3983,7 +3989,7 @@
         <v>306</v>
       </c>
       <c r="J38" s="2" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="K38" s="5">
         <v>0</v>
@@ -4018,7 +4024,7 @@
         <v>32</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="H39" s="2" t="s">
         <v>306</v>
@@ -4027,7 +4033,7 @@
         <v>306</v>
       </c>
       <c r="J39" s="2" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="K39" s="5">
         <v>0</v>
@@ -4062,7 +4068,7 @@
         <v>13</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="H40" s="2" t="s">
         <v>306</v>
@@ -4071,7 +4077,7 @@
         <v>306</v>
       </c>
       <c r="J40" s="2" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="K40" s="5">
         <v>0</v>
@@ -4106,7 +4112,7 @@
         <v>10</v>
       </c>
       <c r="G41" s="2" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="H41" s="2" t="s">
         <v>306</v>
@@ -4115,7 +4121,7 @@
         <v>306</v>
       </c>
       <c r="J41" s="2" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="K41" s="5">
         <v>0</v>
@@ -4150,7 +4156,7 @@
         <v>6</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="H42" s="2" t="s">
         <v>306</v>
@@ -4159,7 +4165,7 @@
         <v>306</v>
       </c>
       <c r="J42" s="2" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="K42" s="5">
         <v>0</v>
@@ -4194,7 +4200,7 @@
         <v>13</v>
       </c>
       <c r="G43" s="2" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="H43" s="2" t="s">
         <v>306</v>
@@ -4203,7 +4209,7 @@
         <v>306</v>
       </c>
       <c r="J43" s="2" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="K43" s="5">
         <v>0</v>
@@ -4238,7 +4244,7 @@
         <v>14</v>
       </c>
       <c r="G44" s="2" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="H44" s="2" t="s">
         <v>306</v>
@@ -4247,7 +4253,7 @@
         <v>306</v>
       </c>
       <c r="J44" s="2" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="K44" s="5">
         <v>0</v>
@@ -4270,7 +4276,7 @@
         <v>324</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="D45" s="2" t="s">
         <v>326</v>
@@ -4282,7 +4288,7 @@
         <v>26</v>
       </c>
       <c r="G45" s="2" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="H45" s="2" t="s">
         <v>306</v>
@@ -4291,7 +4297,7 @@
         <v>306</v>
       </c>
       <c r="J45" s="2" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="K45" s="5">
         <v>0</v>
@@ -4307,134 +4313,178 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="19.5" customFormat="1" s="1">
-      <c r="A46" s="16" t="s">
-        <v>455</v>
-      </c>
-      <c r="B46" s="16" t="s">
+      <c r="A46" s="14" t="s">
         <v>456</v>
       </c>
-      <c r="C46" s="16" t="s">
+      <c r="B46" s="14" t="s">
         <v>457</v>
       </c>
-      <c r="D46" s="16" t="s">
+      <c r="C46" s="14" t="s">
+        <v>458</v>
+      </c>
+      <c r="D46" s="14" t="s">
         <v>326</v>
       </c>
-      <c r="E46" s="16" t="s">
+      <c r="E46" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="F46" s="17">
+      <c r="F46" s="15">
         <v>11</v>
       </c>
-      <c r="G46" s="16" t="s">
-        <v>458</v>
-      </c>
-      <c r="H46" s="16" t="s">
-        <v>306</v>
-      </c>
-      <c r="I46" s="16" t="s">
-        <v>306</v>
-      </c>
-      <c r="J46" s="16" t="s">
-        <v>408</v>
-      </c>
-      <c r="K46" s="17">
-        <v>0</v>
-      </c>
-      <c r="L46" s="17">
-        <v>0</v>
-      </c>
-      <c r="M46" s="17">
-        <v>0</v>
-      </c>
-      <c r="N46" s="17">
+      <c r="G46" s="14" t="s">
+        <v>459</v>
+      </c>
+      <c r="H46" s="14" t="s">
+        <v>306</v>
+      </c>
+      <c r="I46" s="14" t="s">
+        <v>306</v>
+      </c>
+      <c r="J46" s="14" t="s">
+        <v>409</v>
+      </c>
+      <c r="K46" s="15">
+        <v>0</v>
+      </c>
+      <c r="L46" s="15">
+        <v>0</v>
+      </c>
+      <c r="M46" s="15">
+        <v>0</v>
+      </c>
+      <c r="N46" s="15">
         <v>0</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="19.5" customFormat="1" s="1">
-      <c r="A47" s="16" t="s">
-        <v>459</v>
-      </c>
-      <c r="B47" s="16" t="s">
+      <c r="A47" s="14" t="s">
         <v>460</v>
       </c>
-      <c r="C47" s="16" t="s">
+      <c r="B47" s="14" t="s">
         <v>461</v>
       </c>
-      <c r="D47" s="16" t="s">
+      <c r="C47" s="14" t="s">
+        <v>462</v>
+      </c>
+      <c r="D47" s="14" t="s">
         <v>326</v>
       </c>
-      <c r="E47" s="16" t="s">
+      <c r="E47" s="14" t="s">
         <v>160</v>
       </c>
-      <c r="F47" s="17">
+      <c r="F47" s="15">
         <v>14</v>
       </c>
-      <c r="G47" s="16" t="s">
-        <v>462</v>
-      </c>
-      <c r="H47" s="16" t="s">
-        <v>306</v>
-      </c>
-      <c r="I47" s="16" t="s">
-        <v>306</v>
-      </c>
-      <c r="J47" s="16" t="s">
-        <v>408</v>
-      </c>
-      <c r="K47" s="17">
-        <v>0</v>
-      </c>
-      <c r="L47" s="17">
-        <v>0</v>
-      </c>
-      <c r="M47" s="17">
-        <v>0</v>
-      </c>
-      <c r="N47" s="17">
-        <v>0</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="19.5" customFormat="1" s="1">
-      <c r="A48" s="4" t="s">
+      <c r="G47" s="14" t="s">
+        <v>463</v>
+      </c>
+      <c r="H47" s="14" t="s">
+        <v>306</v>
+      </c>
+      <c r="I47" s="14" t="s">
+        <v>306</v>
+      </c>
+      <c r="J47" s="14" t="s">
+        <v>409</v>
+      </c>
+      <c r="K47" s="15">
+        <v>0</v>
+      </c>
+      <c r="L47" s="15">
+        <v>0</v>
+      </c>
+      <c r="M47" s="15">
+        <v>0</v>
+      </c>
+      <c r="N47" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="19.5">
+      <c r="A48" s="16" t="s">
+        <v>464</v>
+      </c>
+      <c r="B48" s="16" t="s">
+        <v>465</v>
+      </c>
+      <c r="C48" s="16" t="s">
+        <v>466</v>
+      </c>
+      <c r="D48" s="16" t="s">
+        <v>467</v>
+      </c>
+      <c r="E48" s="16" t="s">
+        <v>327</v>
+      </c>
+      <c r="F48" s="17">
+        <v>17</v>
+      </c>
+      <c r="G48" s="16" t="s">
+        <v>468</v>
+      </c>
+      <c r="H48" s="16" t="s">
+        <v>306</v>
+      </c>
+      <c r="I48" s="16" t="s">
+        <v>306</v>
+      </c>
+      <c r="J48" s="16" t="s">
+        <v>409</v>
+      </c>
+      <c r="K48" s="17">
+        <v>0</v>
+      </c>
+      <c r="L48" s="17">
+        <v>0</v>
+      </c>
+      <c r="M48" s="17">
+        <v>0</v>
+      </c>
+      <c r="N48" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="19.5" customFormat="1" s="1">
+      <c r="A49" s="4" t="s">
         <v>332</v>
       </c>
-      <c r="B48" s="2" t="s">
+      <c r="B49" s="2" t="s">
         <v>333</v>
       </c>
-      <c r="C48" s="2" t="s">
-        <v>463</v>
-      </c>
-      <c r="D48" s="2" t="s">
+      <c r="C49" s="2" t="s">
+        <v>469</v>
+      </c>
+      <c r="D49" s="2" t="s">
         <v>326</v>
       </c>
-      <c r="E48" s="2" t="s">
+      <c r="E49" s="2" t="s">
         <v>327</v>
       </c>
-      <c r="F48" s="5">
+      <c r="F49" s="5">
         <v>43</v>
       </c>
-      <c r="G48" s="2" t="s">
-        <v>464</v>
-      </c>
-      <c r="H48" s="2" t="s">
-        <v>306</v>
-      </c>
-      <c r="I48" s="2" t="s">
-        <v>306</v>
-      </c>
-      <c r="J48" s="2" t="s">
-        <v>408</v>
-      </c>
-      <c r="K48" s="5">
-        <v>0</v>
-      </c>
-      <c r="L48" s="5">
-        <v>0</v>
-      </c>
-      <c r="M48" s="5">
-        <v>0</v>
-      </c>
-      <c r="N48" s="5">
+      <c r="G49" s="2" t="s">
+        <v>470</v>
+      </c>
+      <c r="H49" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="I49" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="J49" s="2" t="s">
+        <v>409</v>
+      </c>
+      <c r="K49" s="5">
+        <v>0</v>
+      </c>
+      <c r="L49" s="5">
+        <v>0</v>
+      </c>
+      <c r="M49" s="5">
+        <v>0</v>
+      </c>
+      <c r="N49" s="5">
         <v>0</v>
       </c>
     </row>
@@ -4454,10 +4504,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="14" width="14.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="15" width="15.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="14" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="14" width="15.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="12" width="14.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="13" width="15.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="12" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="12" width="15.43357142857143" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
@@ -4607,39 +4657,33 @@
       <c r="B11" s="8" t="s">
         <v>380</v>
       </c>
-      <c r="C11" s="11" t="s">
+      <c r="C11" s="8"/>
+      <c r="D11" s="8" t="s">
         <v>381</v>
-      </c>
-      <c r="D11" s="8" t="s">
-        <v>382</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
       <c r="A12" s="8" t="s">
+        <v>382</v>
+      </c>
+      <c r="B12" s="8" t="s">
         <v>383</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="C12" s="8"/>
+      <c r="D12" s="8" t="s">
         <v>384</v>
-      </c>
-      <c r="C12" s="11" t="s">
-        <v>381</v>
-      </c>
-      <c r="D12" s="8" t="s">
-        <v>385</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
       <c r="A13" s="10" t="s">
+        <v>385</v>
+      </c>
+      <c r="B13" s="8" t="s">
         <v>386</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="C13" s="8"/>
+      <c r="D13" s="8" t="s">
         <v>387</v>
-      </c>
-      <c r="C13" s="11" t="s">
-        <v>381</v>
-      </c>
-      <c r="D13" s="11" t="s">
-        <v>381</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
@@ -4649,156 +4693,104 @@
       <c r="B14" s="8" t="s">
         <v>389</v>
       </c>
-      <c r="C14" s="11" t="s">
-        <v>381</v>
-      </c>
-      <c r="D14" s="11" t="s">
-        <v>381</v>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8" t="s">
+        <v>390</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
       <c r="A15" s="10" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>391</v>
-      </c>
-      <c r="C15" s="11" t="s">
-        <v>381</v>
-      </c>
-      <c r="D15" s="11" t="s">
-        <v>381</v>
-      </c>
+        <v>392</v>
+      </c>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
       <c r="A16" s="10" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>393</v>
-      </c>
-      <c r="C16" s="11" t="s">
-        <v>381</v>
-      </c>
-      <c r="D16" s="11" t="s">
-        <v>381</v>
-      </c>
+        <v>394</v>
+      </c>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
-      <c r="A17" s="11" t="s">
-        <v>381</v>
-      </c>
-      <c r="B17" s="11" t="s">
-        <v>381</v>
-      </c>
+      <c r="A17" s="8"/>
+      <c r="B17" s="8"/>
       <c r="C17" s="10"/>
-      <c r="D17" s="11" t="s">
-        <v>381</v>
-      </c>
+      <c r="D17" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
       <c r="A18" s="8" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="C18" s="10"/>
-      <c r="D18" s="11" t="s">
-        <v>381</v>
-      </c>
+      <c r="D18" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5">
       <c r="A19" s="8" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="C19" s="10"/>
-      <c r="D19" s="12" t="s">
-        <v>381</v>
-      </c>
+      <c r="D19" s="10"/>
     </row>
     <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5">
-      <c r="A20" s="12" t="s">
-        <v>381</v>
-      </c>
+      <c r="A20" s="10"/>
       <c r="B20" s="8" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="C20" s="10"/>
-      <c r="D20" s="12" t="s">
-        <v>381</v>
-      </c>
+      <c r="D20" s="10"/>
     </row>
     <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="19.5">
-      <c r="A21" s="11" t="s">
-        <v>381</v>
-      </c>
+      <c r="A21" s="8"/>
       <c r="B21" s="8" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="C21" s="10"/>
-      <c r="D21" s="12" t="s">
-        <v>381</v>
-      </c>
+      <c r="D21" s="10"/>
     </row>
     <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="19.5">
-      <c r="A22" s="11" t="s">
-        <v>381</v>
-      </c>
+      <c r="A22" s="8"/>
       <c r="B22" s="8" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="C22" s="10"/>
-      <c r="D22" s="12" t="s">
-        <v>381</v>
-      </c>
+      <c r="D22" s="10"/>
     </row>
     <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="19.5">
-      <c r="A23" s="11" t="s">
-        <v>381</v>
-      </c>
-      <c r="B23" s="11" t="s">
-        <v>381</v>
-      </c>
+      <c r="A23" s="8"/>
+      <c r="B23" s="8"/>
       <c r="C23" s="10"/>
-      <c r="D23" s="12" t="s">
-        <v>381</v>
-      </c>
+      <c r="D23" s="10"/>
     </row>
     <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="19.5">
-      <c r="A24" s="12" t="s">
-        <v>381</v>
-      </c>
-      <c r="B24" s="11" t="s">
-        <v>381</v>
-      </c>
+      <c r="A24" s="10"/>
+      <c r="B24" s="8"/>
       <c r="C24" s="10"/>
-      <c r="D24" s="12" t="s">
-        <v>381</v>
-      </c>
+      <c r="D24" s="10"/>
     </row>
     <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="19.5">
       <c r="A25" s="10"/>
-      <c r="B25" s="13" t="s">
-        <v>381</v>
-      </c>
+      <c r="B25" s="11"/>
       <c r="C25" s="10"/>
       <c r="D25" s="10"/>
     </row>
     <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75">
-      <c r="A26" s="12" t="s">
-        <v>381</v>
-      </c>
-      <c r="B26" s="11" t="s">
-        <v>381</v>
-      </c>
+      <c r="A26" s="10"/>
+      <c r="B26" s="8"/>
       <c r="C26" s="10"/>
-      <c r="D26" s="12" t="s">
-        <v>381</v>
-      </c>
+      <c r="D26" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
now with player data lookup
</commit_message>
<xml_diff>
--- a/SJ Fall 2022 (Oct3- Dec23) Tournaments.xlsx
+++ b/SJ Fall 2022 (Oct3- Dec23) Tournaments.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="990" uniqueCount="482">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="992" uniqueCount="484">
   <si>
     <t>fullLink</t>
   </si>
@@ -1162,6 +1162,9 @@
     <t>Hoodinii</t>
   </si>
   <si>
+    <t>BorknBeans</t>
+  </si>
+  <si>
     <t>Yeast</t>
   </si>
   <si>
@@ -1196,6 +1199,9 @@
   </si>
   <si>
     <t>Treestain</t>
+  </si>
+  <si>
+    <t>NicoNico</t>
   </si>
   <si>
     <t>haze</t>
@@ -1493,13 +1499,13 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF000000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -1656,16 +1662,16 @@
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="5" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
@@ -2040,11 +2046,11 @@
         <v>289</v>
       </c>
       <c r="G1" s="24" t="s">
-        <v>467</v>
+        <v>469</v>
       </c>
       <c r="H1" s="14"/>
       <c r="I1" s="25" t="s">
-        <v>471</v>
+        <v>473</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="72" customFormat="1" s="1">
@@ -2071,7 +2077,7 @@
       </c>
       <c r="H2" s="14"/>
       <c r="I2" s="26" t="s">
-        <v>472</v>
+        <v>474</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="85.5" customFormat="1" s="1">
@@ -2098,7 +2104,7 @@
       </c>
       <c r="H3" s="14"/>
       <c r="I3" s="26" t="s">
-        <v>473</v>
+        <v>475</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="72" customFormat="1" s="1">
@@ -2123,7 +2129,7 @@
       <c r="G4" s="2"/>
       <c r="H4" s="14"/>
       <c r="I4" s="26" t="s">
-        <v>474</v>
+        <v>476</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="72">
@@ -2145,10 +2151,10 @@
       </c>
       <c r="G5" s="2"/>
       <c r="H5" s="8" t="s">
-        <v>475</v>
+        <v>477</v>
       </c>
       <c r="I5" s="26" t="s">
-        <v>476</v>
+        <v>478</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="66" customFormat="1" s="1">
@@ -2171,7 +2177,7 @@
       <c r="G6" s="2"/>
       <c r="H6" s="14"/>
       <c r="I6" s="28" t="s">
-        <v>477</v>
+        <v>479</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="78" customFormat="1" s="1">
@@ -2190,7 +2196,7 @@
       <c r="G7" s="2"/>
       <c r="H7" s="14"/>
       <c r="I7" s="28" t="s">
-        <v>478</v>
+        <v>480</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="66" customFormat="1" s="1">
@@ -2209,7 +2215,7 @@
       <c r="G8" s="2"/>
       <c r="H8" s="14"/>
       <c r="I8" s="28" t="s">
-        <v>479</v>
+        <v>481</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="66" customFormat="1" s="1">
@@ -2228,7 +2234,7 @@
       <c r="G9" s="2"/>
       <c r="H9" s="14"/>
       <c r="I9" s="26" t="s">
-        <v>480</v>
+        <v>482</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="66" customFormat="1" s="1">
@@ -2245,7 +2251,7 @@
       <c r="G10" s="2"/>
       <c r="H10" s="14"/>
       <c r="I10" s="26" t="s">
-        <v>481</v>
+        <v>483</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="66" customFormat="1" s="1">
@@ -2334,16 +2340,16 @@
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="32.25" customFormat="1" s="1">
       <c r="A1" s="2" t="s">
-        <v>402</v>
+        <v>404</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>403</v>
+        <v>405</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>4</v>
@@ -2352,7 +2358,7 @@
         <v>5</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>406</v>
+        <v>408</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>7</v>
@@ -2373,7 +2379,7 @@
         <v>12</v>
       </c>
       <c r="N1" s="3" t="s">
-        <v>407</v>
+        <v>409</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="138" customFormat="1" s="1">
@@ -2396,7 +2402,7 @@
         <v>21</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>408</v>
+        <v>410</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>306</v>
@@ -2405,7 +2411,7 @@
         <v>306</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>409</v>
+        <v>411</v>
       </c>
       <c r="K2" s="5">
         <v>0</v>
@@ -2440,7 +2446,7 @@
         <v>13</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>410</v>
+        <v>412</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>306</v>
@@ -2449,7 +2455,7 @@
         <v>306</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>409</v>
+        <v>411</v>
       </c>
       <c r="K3" s="5">
         <v>0</v>
@@ -2484,16 +2490,16 @@
         <v>8</v>
       </c>
       <c r="G4" s="2" t="s">
+        <v>413</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="J4" s="2" t="s">
         <v>411</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>306</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>306</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>409</v>
       </c>
       <c r="K4" s="5">
         <v>0</v>
@@ -2516,7 +2522,7 @@
         <v>37</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>412</v>
+        <v>414</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>16</v>
@@ -2528,7 +2534,7 @@
         <v>7</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>413</v>
+        <v>415</v>
       </c>
       <c r="H5" s="2" t="s">
         <v>306</v>
@@ -2537,7 +2543,7 @@
         <v>306</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>409</v>
+        <v>411</v>
       </c>
       <c r="K5" s="5">
         <v>0</v>
@@ -2560,7 +2566,7 @@
         <v>44</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>414</v>
+        <v>416</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>16</v>
@@ -2572,7 +2578,7 @@
         <v>20</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>415</v>
+        <v>417</v>
       </c>
       <c r="H6" s="2" t="s">
         <v>306</v>
@@ -2581,7 +2587,7 @@
         <v>306</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>409</v>
+        <v>411</v>
       </c>
       <c r="K6" s="5">
         <v>0</v>
@@ -2616,7 +2622,7 @@
         <v>10</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>416</v>
+        <v>418</v>
       </c>
       <c r="H7" s="2" t="s">
         <v>306</v>
@@ -2625,7 +2631,7 @@
         <v>306</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>409</v>
+        <v>411</v>
       </c>
       <c r="K7" s="5">
         <v>0</v>
@@ -2660,7 +2666,7 @@
         <v>9</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>417</v>
+        <v>419</v>
       </c>
       <c r="H8" s="2" t="s">
         <v>306</v>
@@ -2669,7 +2675,7 @@
         <v>306</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>409</v>
+        <v>411</v>
       </c>
       <c r="K8" s="5">
         <v>0</v>
@@ -2704,7 +2710,7 @@
         <v>6</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>418</v>
+        <v>420</v>
       </c>
       <c r="H9" s="2" t="s">
         <v>306</v>
@@ -2713,7 +2719,7 @@
         <v>306</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>409</v>
+        <v>411</v>
       </c>
       <c r="K9" s="5">
         <v>0</v>
@@ -2748,7 +2754,7 @@
         <v>11</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>419</v>
+        <v>421</v>
       </c>
       <c r="H10" s="2" t="s">
         <v>306</v>
@@ -2757,7 +2763,7 @@
         <v>306</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>409</v>
+        <v>411</v>
       </c>
       <c r="K10" s="5">
         <v>0</v>
@@ -2792,7 +2798,7 @@
         <v>9</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>420</v>
+        <v>422</v>
       </c>
       <c r="H11" s="2" t="s">
         <v>306</v>
@@ -2801,7 +2807,7 @@
         <v>306</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>409</v>
+        <v>411</v>
       </c>
       <c r="K11" s="5">
         <v>0</v>
@@ -2836,7 +2842,7 @@
         <v>21</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>421</v>
+        <v>423</v>
       </c>
       <c r="H12" s="2" t="s">
         <v>306</v>
@@ -2845,7 +2851,7 @@
         <v>306</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>409</v>
+        <v>411</v>
       </c>
       <c r="K12" s="5">
         <v>0</v>
@@ -2880,7 +2886,7 @@
         <v>10</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>422</v>
+        <v>424</v>
       </c>
       <c r="H13" s="2" t="s">
         <v>306</v>
@@ -2889,7 +2895,7 @@
         <v>306</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>409</v>
+        <v>411</v>
       </c>
       <c r="K13" s="5">
         <v>0</v>
@@ -2924,7 +2930,7 @@
         <v>8</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>423</v>
+        <v>425</v>
       </c>
       <c r="H14" s="2" t="s">
         <v>306</v>
@@ -2933,7 +2939,7 @@
         <v>306</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>409</v>
+        <v>411</v>
       </c>
       <c r="K14" s="5">
         <v>0</v>
@@ -2968,7 +2974,7 @@
         <v>7</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>424</v>
+        <v>426</v>
       </c>
       <c r="H15" s="2" t="s">
         <v>306</v>
@@ -2977,7 +2983,7 @@
         <v>306</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>409</v>
+        <v>411</v>
       </c>
       <c r="K15" s="5">
         <v>0</v>
@@ -3012,7 +3018,7 @@
         <v>8</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>425</v>
+        <v>427</v>
       </c>
       <c r="H16" s="2" t="s">
         <v>306</v>
@@ -3021,7 +3027,7 @@
         <v>306</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>409</v>
+        <v>411</v>
       </c>
       <c r="K16" s="5">
         <v>0</v>
@@ -3056,7 +3062,7 @@
         <v>12</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>426</v>
+        <v>428</v>
       </c>
       <c r="H17" s="2" t="s">
         <v>306</v>
@@ -3065,7 +3071,7 @@
         <v>306</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>409</v>
+        <v>411</v>
       </c>
       <c r="K17" s="5">
         <v>0</v>
@@ -3100,7 +3106,7 @@
         <v>20</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>427</v>
+        <v>429</v>
       </c>
       <c r="H18" s="2" t="s">
         <v>306</v>
@@ -3109,7 +3115,7 @@
         <v>306</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>409</v>
+        <v>411</v>
       </c>
       <c r="K18" s="5">
         <v>0</v>
@@ -3144,7 +3150,7 @@
         <v>27</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>428</v>
+        <v>430</v>
       </c>
       <c r="H19" s="2" t="s">
         <v>306</v>
@@ -3153,7 +3159,7 @@
         <v>306</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>409</v>
+        <v>411</v>
       </c>
       <c r="K19" s="5">
         <v>0</v>
@@ -3188,7 +3194,7 @@
         <v>21</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>429</v>
+        <v>431</v>
       </c>
       <c r="H20" s="2" t="s">
         <v>306</v>
@@ -3197,7 +3203,7 @@
         <v>306</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>409</v>
+        <v>411</v>
       </c>
       <c r="K20" s="5">
         <v>0</v>
@@ -3232,7 +3238,7 @@
         <v>32</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>430</v>
+        <v>432</v>
       </c>
       <c r="H21" s="2" t="s">
         <v>306</v>
@@ -3241,7 +3247,7 @@
         <v>306</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>409</v>
+        <v>411</v>
       </c>
       <c r="K21" s="5">
         <v>0</v>
@@ -3276,7 +3282,7 @@
         <v>14</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>431</v>
+        <v>433</v>
       </c>
       <c r="H22" s="2" t="s">
         <v>306</v>
@@ -3285,7 +3291,7 @@
         <v>306</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>409</v>
+        <v>411</v>
       </c>
       <c r="K22" s="5">
         <v>0</v>
@@ -3320,7 +3326,7 @@
         <v>12</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>432</v>
+        <v>434</v>
       </c>
       <c r="H23" s="2" t="s">
         <v>306</v>
@@ -3329,7 +3335,7 @@
         <v>306</v>
       </c>
       <c r="J23" s="2" t="s">
-        <v>409</v>
+        <v>411</v>
       </c>
       <c r="K23" s="5">
         <v>0</v>
@@ -3364,7 +3370,7 @@
         <v>18</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>433</v>
+        <v>435</v>
       </c>
       <c r="H24" s="2" t="s">
         <v>306</v>
@@ -3373,7 +3379,7 @@
         <v>306</v>
       </c>
       <c r="J24" s="2" t="s">
-        <v>409</v>
+        <v>411</v>
       </c>
       <c r="K24" s="5">
         <v>0</v>
@@ -3408,7 +3414,7 @@
         <v>19</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>434</v>
+        <v>436</v>
       </c>
       <c r="H25" s="2" t="s">
         <v>306</v>
@@ -3417,7 +3423,7 @@
         <v>306</v>
       </c>
       <c r="J25" s="2" t="s">
-        <v>409</v>
+        <v>411</v>
       </c>
       <c r="K25" s="5">
         <v>0</v>
@@ -3452,7 +3458,7 @@
         <v>15</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>435</v>
+        <v>437</v>
       </c>
       <c r="H26" s="2" t="s">
         <v>306</v>
@@ -3461,7 +3467,7 @@
         <v>306</v>
       </c>
       <c r="J26" s="2" t="s">
-        <v>409</v>
+        <v>411</v>
       </c>
       <c r="K26" s="5">
         <v>0</v>
@@ -3496,7 +3502,7 @@
         <v>16</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>436</v>
+        <v>438</v>
       </c>
       <c r="H27" s="2" t="s">
         <v>306</v>
@@ -3505,7 +3511,7 @@
         <v>306</v>
       </c>
       <c r="J27" s="2" t="s">
-        <v>409</v>
+        <v>411</v>
       </c>
       <c r="K27" s="5">
         <v>0</v>
@@ -3540,7 +3546,7 @@
         <v>14</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>437</v>
+        <v>439</v>
       </c>
       <c r="H28" s="2" t="s">
         <v>306</v>
@@ -3549,7 +3555,7 @@
         <v>306</v>
       </c>
       <c r="J28" s="2" t="s">
-        <v>409</v>
+        <v>411</v>
       </c>
       <c r="K28" s="5">
         <v>0</v>
@@ -3584,7 +3590,7 @@
         <v>16</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>438</v>
+        <v>440</v>
       </c>
       <c r="H29" s="2" t="s">
         <v>306</v>
@@ -3593,7 +3599,7 @@
         <v>306</v>
       </c>
       <c r="J29" s="2" t="s">
-        <v>409</v>
+        <v>411</v>
       </c>
       <c r="K29" s="5">
         <v>0</v>
@@ -3628,7 +3634,7 @@
         <v>13</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>439</v>
+        <v>441</v>
       </c>
       <c r="H30" s="2" t="s">
         <v>306</v>
@@ -3637,7 +3643,7 @@
         <v>306</v>
       </c>
       <c r="J30" s="2" t="s">
-        <v>409</v>
+        <v>411</v>
       </c>
       <c r="K30" s="5">
         <v>0</v>
@@ -3672,7 +3678,7 @@
         <v>16</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>440</v>
+        <v>442</v>
       </c>
       <c r="H31" s="2" t="s">
         <v>306</v>
@@ -3681,7 +3687,7 @@
         <v>306</v>
       </c>
       <c r="J31" s="2" t="s">
-        <v>409</v>
+        <v>411</v>
       </c>
       <c r="K31" s="5">
         <v>0</v>
@@ -3716,7 +3722,7 @@
         <v>39</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>441</v>
+        <v>443</v>
       </c>
       <c r="H32" s="2" t="s">
         <v>306</v>
@@ -3725,7 +3731,7 @@
         <v>306</v>
       </c>
       <c r="J32" s="2" t="s">
-        <v>409</v>
+        <v>411</v>
       </c>
       <c r="K32" s="5">
         <v>0</v>
@@ -3760,7 +3766,7 @@
         <v>40</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>442</v>
+        <v>444</v>
       </c>
       <c r="H33" s="2" t="s">
         <v>306</v>
@@ -3769,7 +3775,7 @@
         <v>306</v>
       </c>
       <c r="J33" s="2" t="s">
-        <v>409</v>
+        <v>411</v>
       </c>
       <c r="K33" s="5">
         <v>0</v>
@@ -3784,7 +3790,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="230.25" customFormat="1" s="1">
       <c r="A34" s="4" t="s">
         <v>244</v>
       </c>
@@ -3804,7 +3810,7 @@
         <v>21</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>443</v>
+        <v>445</v>
       </c>
       <c r="H34" s="2" t="s">
         <v>306</v>
@@ -3813,7 +3819,7 @@
         <v>306</v>
       </c>
       <c r="J34" s="2" t="s">
-        <v>409</v>
+        <v>411</v>
       </c>
       <c r="K34" s="5">
         <v>0</v>
@@ -3828,7 +3834,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="322.5" customFormat="1" s="1">
       <c r="A35" s="4" t="s">
         <v>251</v>
       </c>
@@ -3848,7 +3854,7 @@
         <v>31</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>444</v>
+        <v>446</v>
       </c>
       <c r="H35" s="2" t="s">
         <v>306</v>
@@ -3857,7 +3863,7 @@
         <v>306</v>
       </c>
       <c r="J35" s="2" t="s">
-        <v>409</v>
+        <v>411</v>
       </c>
       <c r="K35" s="5">
         <v>0</v>
@@ -3872,7 +3878,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="322.5" customFormat="1" s="1">
       <c r="A36" s="4" t="s">
         <v>258</v>
       </c>
@@ -3892,7 +3898,7 @@
         <v>30</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>445</v>
+        <v>447</v>
       </c>
       <c r="H36" s="2" t="s">
         <v>306</v>
@@ -3901,7 +3907,7 @@
         <v>306</v>
       </c>
       <c r="J36" s="2" t="s">
-        <v>409</v>
+        <v>411</v>
       </c>
       <c r="K36" s="5">
         <v>0</v>
@@ -3916,7 +3922,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="296.25" customFormat="1" s="1">
       <c r="A37" s="4" t="s">
         <v>265</v>
       </c>
@@ -3936,7 +3942,7 @@
         <v>33</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>446</v>
+        <v>448</v>
       </c>
       <c r="H37" s="2" t="s">
         <v>306</v>
@@ -3945,7 +3951,7 @@
         <v>306</v>
       </c>
       <c r="J37" s="2" t="s">
-        <v>409</v>
+        <v>411</v>
       </c>
       <c r="K37" s="5">
         <v>0</v>
@@ -3960,7 +3966,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="270" customFormat="1" s="1">
       <c r="A38" s="4" t="s">
         <v>272</v>
       </c>
@@ -3980,7 +3986,7 @@
         <v>26</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>447</v>
+        <v>449</v>
       </c>
       <c r="H38" s="2" t="s">
         <v>306</v>
@@ -3989,7 +3995,7 @@
         <v>306</v>
       </c>
       <c r="J38" s="2" t="s">
-        <v>409</v>
+        <v>411</v>
       </c>
       <c r="K38" s="5">
         <v>0</v>
@@ -4004,7 +4010,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="336" customFormat="1" s="1">
       <c r="A39" s="4" t="s">
         <v>279</v>
       </c>
@@ -4024,7 +4030,7 @@
         <v>32</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>448</v>
+        <v>450</v>
       </c>
       <c r="H39" s="2" t="s">
         <v>306</v>
@@ -4033,7 +4039,7 @@
         <v>306</v>
       </c>
       <c r="J39" s="2" t="s">
-        <v>409</v>
+        <v>411</v>
       </c>
       <c r="K39" s="5">
         <v>0</v>
@@ -4048,7 +4054,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="124.5" customFormat="1" s="1">
       <c r="A40" s="4" t="s">
         <v>286</v>
       </c>
@@ -4068,7 +4074,7 @@
         <v>13</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>449</v>
+        <v>451</v>
       </c>
       <c r="H40" s="2" t="s">
         <v>306</v>
@@ -4077,7 +4083,7 @@
         <v>306</v>
       </c>
       <c r="J40" s="2" t="s">
-        <v>409</v>
+        <v>411</v>
       </c>
       <c r="K40" s="5">
         <v>0</v>
@@ -4092,7 +4098,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="98.25" customFormat="1" s="1">
       <c r="A41" s="4" t="s">
         <v>295</v>
       </c>
@@ -4112,7 +4118,7 @@
         <v>10</v>
       </c>
       <c r="G41" s="2" t="s">
-        <v>450</v>
+        <v>452</v>
       </c>
       <c r="H41" s="2" t="s">
         <v>306</v>
@@ -4121,7 +4127,7 @@
         <v>306</v>
       </c>
       <c r="J41" s="2" t="s">
-        <v>409</v>
+        <v>411</v>
       </c>
       <c r="K41" s="5">
         <v>0</v>
@@ -4136,7 +4142,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="85.5" customFormat="1" s="1">
       <c r="A42" s="4" t="s">
         <v>302</v>
       </c>
@@ -4156,7 +4162,7 @@
         <v>6</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>451</v>
+        <v>453</v>
       </c>
       <c r="H42" s="2" t="s">
         <v>306</v>
@@ -4165,7 +4171,7 @@
         <v>306</v>
       </c>
       <c r="J42" s="2" t="s">
-        <v>409</v>
+        <v>411</v>
       </c>
       <c r="K42" s="5">
         <v>0</v>
@@ -4180,7 +4186,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="138" customFormat="1" s="1">
       <c r="A43" s="4" t="s">
         <v>309</v>
       </c>
@@ -4200,7 +4206,7 @@
         <v>13</v>
       </c>
       <c r="G43" s="2" t="s">
-        <v>452</v>
+        <v>454</v>
       </c>
       <c r="H43" s="2" t="s">
         <v>306</v>
@@ -4209,7 +4215,7 @@
         <v>306</v>
       </c>
       <c r="J43" s="2" t="s">
-        <v>409</v>
+        <v>411</v>
       </c>
       <c r="K43" s="5">
         <v>0</v>
@@ -4224,7 +4230,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="138" customFormat="1" s="1">
       <c r="A44" s="4" t="s">
         <v>316</v>
       </c>
@@ -4244,7 +4250,7 @@
         <v>14</v>
       </c>
       <c r="G44" s="2" t="s">
-        <v>453</v>
+        <v>455</v>
       </c>
       <c r="H44" s="2" t="s">
         <v>306</v>
@@ -4253,7 +4259,7 @@
         <v>306</v>
       </c>
       <c r="J44" s="2" t="s">
-        <v>409</v>
+        <v>411</v>
       </c>
       <c r="K44" s="5">
         <v>0</v>
@@ -4268,7 +4274,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="256.5" customFormat="1" s="1">
       <c r="A45" s="4" t="s">
         <v>323</v>
       </c>
@@ -4276,7 +4282,7 @@
         <v>324</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>454</v>
+        <v>456</v>
       </c>
       <c r="D45" s="2" t="s">
         <v>326</v>
@@ -4288,7 +4294,7 @@
         <v>26</v>
       </c>
       <c r="G45" s="2" t="s">
-        <v>455</v>
+        <v>457</v>
       </c>
       <c r="H45" s="2" t="s">
         <v>306</v>
@@ -4297,7 +4303,7 @@
         <v>306</v>
       </c>
       <c r="J45" s="2" t="s">
-        <v>409</v>
+        <v>411</v>
       </c>
       <c r="K45" s="5">
         <v>0</v>
@@ -4312,15 +4318,15 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="116.25" customFormat="1" s="1">
       <c r="A46" s="14" t="s">
-        <v>456</v>
+        <v>458</v>
       </c>
       <c r="B46" s="14" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
       <c r="C46" s="14" t="s">
-        <v>458</v>
+        <v>460</v>
       </c>
       <c r="D46" s="14" t="s">
         <v>326</v>
@@ -4332,7 +4338,7 @@
         <v>11</v>
       </c>
       <c r="G46" s="14" t="s">
-        <v>459</v>
+        <v>461</v>
       </c>
       <c r="H46" s="14" t="s">
         <v>306</v>
@@ -4341,7 +4347,7 @@
         <v>306</v>
       </c>
       <c r="J46" s="14" t="s">
-        <v>409</v>
+        <v>411</v>
       </c>
       <c r="K46" s="15">
         <v>0</v>
@@ -4356,15 +4362,15 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="144" customFormat="1" s="1">
       <c r="A47" s="14" t="s">
-        <v>460</v>
+        <v>462</v>
       </c>
       <c r="B47" s="14" t="s">
-        <v>461</v>
+        <v>463</v>
       </c>
       <c r="C47" s="14" t="s">
-        <v>462</v>
+        <v>464</v>
       </c>
       <c r="D47" s="14" t="s">
         <v>326</v>
@@ -4376,7 +4382,7 @@
         <v>14</v>
       </c>
       <c r="G47" s="14" t="s">
-        <v>463</v>
+        <v>465</v>
       </c>
       <c r="H47" s="14" t="s">
         <v>306</v>
@@ -4385,7 +4391,7 @@
         <v>306</v>
       </c>
       <c r="J47" s="14" t="s">
-        <v>409</v>
+        <v>411</v>
       </c>
       <c r="K47" s="15">
         <v>0</v>
@@ -4400,18 +4406,18 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="151.5" customFormat="1" s="1">
       <c r="A48" s="16" t="s">
-        <v>464</v>
+        <v>466</v>
       </c>
       <c r="B48" s="16" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="C48" s="16" t="s">
-        <v>466</v>
+        <v>468</v>
       </c>
       <c r="D48" s="16" t="s">
-        <v>467</v>
+        <v>469</v>
       </c>
       <c r="E48" s="16" t="s">
         <v>327</v>
@@ -4420,7 +4426,7 @@
         <v>17</v>
       </c>
       <c r="G48" s="16" t="s">
-        <v>468</v>
+        <v>470</v>
       </c>
       <c r="H48" s="16" t="s">
         <v>306</v>
@@ -4429,7 +4435,7 @@
         <v>306</v>
       </c>
       <c r="J48" s="16" t="s">
-        <v>409</v>
+        <v>411</v>
       </c>
       <c r="K48" s="17">
         <v>0</v>
@@ -4444,7 +4450,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="402" customFormat="1" s="1">
       <c r="A49" s="4" t="s">
         <v>332</v>
       </c>
@@ -4452,7 +4458,7 @@
         <v>333</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>469</v>
+        <v>471</v>
       </c>
       <c r="D49" s="2" t="s">
         <v>326</v>
@@ -4464,7 +4470,7 @@
         <v>43</v>
       </c>
       <c r="G49" s="2" t="s">
-        <v>470</v>
+        <v>472</v>
       </c>
       <c r="H49" s="2" t="s">
         <v>306</v>
@@ -4473,7 +4479,7 @@
         <v>306</v>
       </c>
       <c r="J49" s="2" t="s">
-        <v>409</v>
+        <v>411</v>
       </c>
       <c r="K49" s="5">
         <v>0</v>
@@ -4657,63 +4663,67 @@
       <c r="B11" s="8" t="s">
         <v>380</v>
       </c>
-      <c r="C11" s="8"/>
+      <c r="C11" s="8" t="s">
+        <v>381</v>
+      </c>
       <c r="D11" s="8" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
       <c r="A12" s="8" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="C12" s="8"/>
       <c r="D12" s="8" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
       <c r="A13" s="10" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="C13" s="8"/>
       <c r="D13" s="8" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
       <c r="A14" s="10" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="C14" s="8"/>
       <c r="D14" s="8" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
       <c r="A15" s="10" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
+      <c r="D15" s="8" t="s">
+        <v>394</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
       <c r="A16" s="10" t="s">
-        <v>393</v>
+        <v>395</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="C16" s="8"/>
       <c r="D16" s="8"/>
@@ -4726,20 +4736,20 @@
     </row>
     <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
       <c r="A18" s="8" t="s">
-        <v>395</v>
+        <v>397</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="C18" s="10"/>
       <c r="D18" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5">
       <c r="A19" s="8" t="s">
-        <v>397</v>
+        <v>399</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>398</v>
+        <v>400</v>
       </c>
       <c r="C19" s="10"/>
       <c r="D19" s="10"/>
@@ -4747,7 +4757,7 @@
     <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5">
       <c r="A20" s="10"/>
       <c r="B20" s="8" t="s">
-        <v>399</v>
+        <v>401</v>
       </c>
       <c r="C20" s="10"/>
       <c r="D20" s="10"/>
@@ -4755,7 +4765,7 @@
     <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="19.5">
       <c r="A21" s="8"/>
       <c r="B21" s="8" t="s">
-        <v>400</v>
+        <v>402</v>
       </c>
       <c r="C21" s="10"/>
       <c r="D21" s="10"/>
@@ -4763,7 +4773,7 @@
     <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="19.5">
       <c r="A22" s="8"/>
       <c r="B22" s="8" t="s">
-        <v>401</v>
+        <v>403</v>
       </c>
       <c r="C22" s="10"/>
       <c r="D22" s="10"/>

</xml_diff>

<commit_message>
large update, with SJ 2023 and an old 2022 q2 stuff
</commit_message>
<xml_diff>
--- a/SJ Fall 2022 (Oct3- Dec23) Tournaments.xlsx
+++ b/SJ Fall 2022 (Oct3- Dec23) Tournaments.xlsx
@@ -4,7 +4,7 @@
   <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="2"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet r:id="rId1" sheetId="1" name="Fall Tourneys"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="999" uniqueCount="488">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1021" uniqueCount="500">
   <si>
     <t>fullLink</t>
   </si>
@@ -1189,9 +1189,6 @@
     <t>DSF</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t>Vince</t>
   </si>
   <si>
@@ -1442,6 +1439,45 @@
   </si>
   <si>
     <t>Aryeh~~~1$$Ls~~~2$$Xavier~~~3$$EO~~~4$$feelingkettle~~~5$$WheeZy~~~5$$SuperYoshi141~~~7$$VINN~~~7$$Vailskibum94~~~9$$Yoshiya Zeper~~~9$$Unown~~~9$$Grey~~~9$$Crimson Ninja~~~13$$Ian~~~13$$MCheese~~~13$$Unown69~~~13$$Yikes~~~17$$</t>
+  </si>
+  <si>
+    <t>start.gg/tournament/hops-stocks-17-march-20th-2023/event/ultimate-singles</t>
+  </si>
+  <si>
+    <t>hops-stocks-17-march-20th-2023</t>
+  </si>
+  <si>
+    <t>Hops N stocks-17-20th-2023</t>
+  </si>
+  <si>
+    <t>Aryeh~~~1$$xavier~~~2$$Noodl~~~3$$A9~~~4$$EO~~~5$$Secret~~~5$$feelingkettle~~~7$$AnVy~~~7$$Consent is Badass~~~9$$Kasugano~~~9$$Conrad~~~9$$koala cub~~~9$$Blackmoon~~~13$$Visada~~~13$$Arcos~~~13$$Kunio~~~13$$ThePsychicBoy~~~17$$Steftendo~~~17$$JACANGIE13~~~17$$</t>
+  </si>
+  <si>
+    <t>start.gg/tournament/battle-over-the-bridge-80/event/ultimate-singles</t>
+  </si>
+  <si>
+    <t>battle-over-the-bridge-80</t>
+  </si>
+  <si>
+    <t>Battle Over The Bridge-80</t>
+  </si>
+  <si>
+    <t>Battle Over the Bridge</t>
+  </si>
+  <si>
+    <t>Hoodinii~~~1$$Aryeh~~~2$$AUSTI~~~3$$feelingkettle~~~4$$Ham Burrito~~~5$$Secret~~~5$$Steftendo~~~7$$PoP~~~7$$Steezus~~~9$$Hackerbot~~~9$$</t>
+  </si>
+  <si>
+    <t>start.gg/tournament/ru-smashin-spring-2023-8/event/ultimate-singles</t>
+  </si>
+  <si>
+    <t>ru-smashin-spring-2023-8</t>
+  </si>
+  <si>
+    <t>RU Smashin-2023-8</t>
+  </si>
+  <si>
+    <t>A9~~~1$$Vince~~~2$$xavier~~~3$$Noodl~~~4$$AUSTI~~~5$$Blase~~~5$$Jesty~~~7$$Joba~~~7$$Spectro~~~9$$Hoodinii~~~9$$Consent is Badass~~~9$$Grey~~~9$$ShyTy~~~13$$Cipher~~~13$$Torrent~~~13$$Loki~~~13$$kino.~~~17$$MMMM~~~17$$acorn~~~17$$Nameless~~~17$$that0neguy~~~17$$ggecko~~~17$$Crest~~~17$$PokemonMasterNick~~~17$$Palabra~~~25$$Calamari~~~25$$Faith~~~25$$ALTAlter~~~25$$Mattchew~~~25$$Taman~~~25$$daddy~~~25$$Nickincho~~~25$$MelonLord~~~33$$MCheese~~~33$$</t>
   </si>
   <si>
     <t>Pbj Holiday Palooza</t>
@@ -1627,7 +1663,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1659,9 +1695,6 @@
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1675,6 +1708,12 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="4" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
@@ -2018,263 +2057,263 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="14" width="15.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="14" width="15.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="14" width="19.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="13" width="15.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="13" width="15.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="13" width="19.576428571428572" customWidth="1" bestFit="1"/>
     <col min="4" max="4" style="6" width="16.005" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="14" width="16.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="14" width="16.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="14" width="20.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="13" width="18.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="13" width="16.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="13" width="16.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="13" width="20.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="12" width="18.719285714285714" customWidth="1" bestFit="1"/>
     <col min="9" max="9" style="6" width="31.14785714285714" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="32.25" customFormat="1" s="1">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="C1" s="20" t="s">
         <v>136</v>
       </c>
-      <c r="D1" s="20" t="s">
+      <c r="D1" s="21" t="s">
         <v>159</v>
       </c>
-      <c r="E1" s="21" t="s">
+      <c r="E1" s="22" t="s">
         <v>231</v>
       </c>
-      <c r="F1" s="22" t="s">
+      <c r="F1" s="23" t="s">
         <v>289</v>
       </c>
-      <c r="G1" s="23" t="s">
-        <v>473</v>
-      </c>
-      <c r="H1" s="15"/>
-      <c r="I1" s="24" t="s">
-        <v>477</v>
+      <c r="G1" s="24" t="s">
+        <v>472</v>
+      </c>
+      <c r="H1" s="14"/>
+      <c r="I1" s="25" t="s">
+        <v>489</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="72" customFormat="1" s="1">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="26" t="s">
         <v>50</v>
       </c>
-      <c r="C2" s="25" t="s">
+      <c r="C2" s="26" t="s">
         <v>133</v>
       </c>
-      <c r="D2" s="25" t="s">
+      <c r="D2" s="26" t="s">
         <v>156</v>
       </c>
-      <c r="E2" s="25" t="s">
+      <c r="E2" s="26" t="s">
         <v>228</v>
       </c>
-      <c r="F2" s="25" t="s">
+      <c r="F2" s="26" t="s">
         <v>286</v>
       </c>
-      <c r="G2" s="25" t="s">
+      <c r="G2" s="26" t="s">
         <v>323</v>
       </c>
-      <c r="H2" s="15"/>
-      <c r="I2" s="25" t="s">
-        <v>478</v>
+      <c r="H2" s="14"/>
+      <c r="I2" s="26" t="s">
+        <v>490</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="85.5" customFormat="1" s="1">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="25" t="s">
+      <c r="B3" s="26" t="s">
         <v>59</v>
       </c>
-      <c r="C3" s="25" t="s">
+      <c r="C3" s="26" t="s">
         <v>142</v>
       </c>
-      <c r="D3" s="25" t="s">
+      <c r="D3" s="26" t="s">
         <v>165</v>
       </c>
-      <c r="E3" s="25" t="s">
+      <c r="E3" s="26" t="s">
         <v>237</v>
       </c>
-      <c r="F3" s="25" t="s">
+      <c r="F3" s="26" t="s">
         <v>295</v>
       </c>
-      <c r="G3" s="25" t="s">
+      <c r="G3" s="26" t="s">
         <v>332</v>
       </c>
-      <c r="H3" s="15"/>
-      <c r="I3" s="25" t="s">
-        <v>479</v>
+      <c r="H3" s="14"/>
+      <c r="I3" s="26" t="s">
+        <v>491</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="72" customFormat="1" s="1">
-      <c r="A4" s="25" t="s">
+      <c r="A4" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="B4" s="25" t="s">
+      <c r="B4" s="26" t="s">
         <v>66</v>
       </c>
-      <c r="C4" s="25" t="s">
+      <c r="C4" s="26" t="s">
         <v>149</v>
       </c>
-      <c r="D4" s="25" t="s">
+      <c r="D4" s="26" t="s">
         <v>172</v>
       </c>
-      <c r="E4" s="25" t="s">
+      <c r="E4" s="26" t="s">
         <v>244</v>
       </c>
-      <c r="F4" s="25" t="s">
+      <c r="F4" s="26" t="s">
         <v>302</v>
       </c>
       <c r="G4" s="2"/>
-      <c r="H4" s="15"/>
-      <c r="I4" s="25" t="s">
-        <v>480</v>
+      <c r="H4" s="14"/>
+      <c r="I4" s="26" t="s">
+        <v>492</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="72">
       <c r="A5" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B5" s="25" t="s">
+      <c r="B5" s="26" t="s">
         <v>73</v>
       </c>
       <c r="C5" s="2"/>
-      <c r="D5" s="25" t="s">
+      <c r="D5" s="26" t="s">
         <v>179</v>
       </c>
-      <c r="E5" s="25" t="s">
+      <c r="E5" s="26" t="s">
         <v>251</v>
       </c>
-      <c r="F5" s="25" t="s">
+      <c r="F5" s="26" t="s">
         <v>309</v>
       </c>
       <c r="G5" s="2"/>
       <c r="H5" s="8" t="s">
-        <v>481</v>
-      </c>
-      <c r="I5" s="25" t="s">
-        <v>482</v>
+        <v>493</v>
+      </c>
+      <c r="I5" s="26" t="s">
+        <v>494</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="66" customFormat="1" s="1">
-      <c r="A6" s="26" t="s">
+      <c r="A6" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="B6" s="25" t="s">
+      <c r="B6" s="26" t="s">
         <v>80</v>
       </c>
       <c r="C6" s="2"/>
-      <c r="D6" s="25" t="s">
+      <c r="D6" s="26" t="s">
         <v>186</v>
       </c>
-      <c r="E6" s="25" t="s">
+      <c r="E6" s="26" t="s">
         <v>258</v>
       </c>
-      <c r="F6" s="25" t="s">
+      <c r="F6" s="26" t="s">
         <v>316</v>
       </c>
       <c r="G6" s="2"/>
-      <c r="H6" s="15"/>
-      <c r="I6" s="27" t="s">
-        <v>483</v>
+      <c r="H6" s="14"/>
+      <c r="I6" s="28" t="s">
+        <v>495</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="78" customFormat="1" s="1">
       <c r="A7" s="2"/>
-      <c r="B7" s="25" t="s">
+      <c r="B7" s="26" t="s">
         <v>86</v>
       </c>
       <c r="C7" s="2"/>
-      <c r="D7" s="25" t="s">
+      <c r="D7" s="26" t="s">
         <v>193</v>
       </c>
-      <c r="E7" s="25" t="s">
+      <c r="E7" s="26" t="s">
         <v>265</v>
       </c>
-      <c r="F7" s="15"/>
+      <c r="F7" s="14"/>
       <c r="G7" s="2"/>
-      <c r="H7" s="15"/>
-      <c r="I7" s="27" t="s">
-        <v>484</v>
+      <c r="H7" s="14"/>
+      <c r="I7" s="28" t="s">
+        <v>496</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="66" customFormat="1" s="1">
       <c r="A8" s="2"/>
-      <c r="B8" s="25" t="s">
+      <c r="B8" s="26" t="s">
         <v>93</v>
       </c>
       <c r="C8" s="2"/>
-      <c r="D8" s="25" t="s">
+      <c r="D8" s="26" t="s">
         <v>200</v>
       </c>
-      <c r="E8" s="25" t="s">
+      <c r="E8" s="26" t="s">
         <v>272</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
-      <c r="H8" s="15"/>
-      <c r="I8" s="27" t="s">
-        <v>485</v>
+      <c r="H8" s="14"/>
+      <c r="I8" s="28" t="s">
+        <v>497</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="66" customFormat="1" s="1">
       <c r="A9" s="2"/>
-      <c r="B9" s="25" t="s">
+      <c r="B9" s="26" t="s">
         <v>99</v>
       </c>
       <c r="C9" s="2"/>
-      <c r="D9" s="25" t="s">
+      <c r="D9" s="26" t="s">
         <v>207</v>
       </c>
-      <c r="E9" s="25" t="s">
+      <c r="E9" s="26" t="s">
         <v>279</v>
       </c>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
-      <c r="H9" s="15"/>
-      <c r="I9" s="25" t="s">
-        <v>486</v>
+      <c r="H9" s="14"/>
+      <c r="I9" s="26" t="s">
+        <v>498</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="66" customFormat="1" s="1">
       <c r="A10" s="2"/>
-      <c r="B10" s="25" t="s">
+      <c r="B10" s="26" t="s">
         <v>106</v>
       </c>
       <c r="C10" s="2"/>
-      <c r="D10" s="25" t="s">
+      <c r="D10" s="26" t="s">
         <v>214</v>
       </c>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
-      <c r="H10" s="15"/>
-      <c r="I10" s="25" t="s">
-        <v>487</v>
+      <c r="H10" s="14"/>
+      <c r="I10" s="26" t="s">
+        <v>499</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="66" customFormat="1" s="1">
       <c r="A11" s="2"/>
-      <c r="B11" s="25" t="s">
+      <c r="B11" s="26" t="s">
         <v>113</v>
       </c>
       <c r="C11" s="2"/>
-      <c r="D11" s="25" t="s">
+      <c r="D11" s="26" t="s">
         <v>221</v>
       </c>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
-      <c r="H11" s="15"/>
-      <c r="I11" s="15"/>
+      <c r="H11" s="14"/>
+      <c r="I11" s="14"/>
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5" customFormat="1" s="1">
       <c r="A12" s="2"/>
-      <c r="B12" s="25" t="s">
+      <c r="B12" s="26" t="s">
         <v>120</v>
       </c>
       <c r="C12" s="2"/>
@@ -2282,12 +2321,12 @@
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
-      <c r="H12" s="15"/>
-      <c r="I12" s="15"/>
+      <c r="H12" s="14"/>
+      <c r="I12" s="14"/>
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5" customFormat="1" s="1">
       <c r="A13" s="2"/>
-      <c r="B13" s="25" t="s">
+      <c r="B13" s="26" t="s">
         <v>126</v>
       </c>
       <c r="C13" s="2"/>
@@ -2295,19 +2334,19 @@
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
-      <c r="H13" s="15"/>
-      <c r="I13" s="15"/>
+      <c r="H13" s="14"/>
+      <c r="I13" s="14"/>
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
       <c r="A14" s="8"/>
       <c r="B14" s="8"/>
       <c r="C14" s="8"/>
-      <c r="D14" s="15"/>
+      <c r="D14" s="14"/>
       <c r="E14" s="8"/>
       <c r="F14" s="8"/>
       <c r="G14" s="8"/>
       <c r="H14" s="10"/>
-      <c r="I14" s="15"/>
+      <c r="I14" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2319,9 +2358,9 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:N49"/>
+  <dimension ref="A1:N52"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2343,16 +2382,16 @@
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="32.25" customFormat="1" s="1">
       <c r="A1" s="2" t="s">
+        <v>405</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>406</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>407</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>408</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>409</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>4</v>
@@ -2361,7 +2400,7 @@
         <v>5</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>7</v>
@@ -2382,10 +2421,10 @@
         <v>12</v>
       </c>
       <c r="N1" s="3" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="138" customFormat="1" s="1">
+        <v>410</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="204" customFormat="1" s="1">
       <c r="A2" s="4" t="s">
         <v>13</v>
       </c>
@@ -2405,17 +2444,17 @@
         <v>21</v>
       </c>
       <c r="G2" s="2" t="s">
+        <v>411</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="J2" s="2" t="s">
         <v>412</v>
       </c>
-      <c r="H2" s="2" t="s">
-        <v>306</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>306</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>413</v>
-      </c>
       <c r="K2" s="5">
         <v>0</v>
       </c>
@@ -2429,7 +2468,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="85.5" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="138" customFormat="1" s="1">
       <c r="A3" s="4" t="s">
         <v>22</v>
       </c>
@@ -2449,7 +2488,7 @@
         <v>13</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>306</v>
@@ -2458,7 +2497,7 @@
         <v>306</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="K3" s="5">
         <v>0</v>
@@ -2493,7 +2532,7 @@
         <v>8</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>306</v>
@@ -2502,7 +2541,7 @@
         <v>306</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="K4" s="5">
         <v>0</v>
@@ -2525,7 +2564,7 @@
         <v>37</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>16</v>
@@ -2537,7 +2576,7 @@
         <v>7</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="H5" s="2" t="s">
         <v>306</v>
@@ -2546,7 +2585,7 @@
         <v>306</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="K5" s="5">
         <v>0</v>
@@ -2569,7 +2608,7 @@
         <v>44</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>16</v>
@@ -2581,7 +2620,7 @@
         <v>20</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="H6" s="2" t="s">
         <v>306</v>
@@ -2590,7 +2629,7 @@
         <v>306</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="K6" s="5">
         <v>0</v>
@@ -2625,7 +2664,7 @@
         <v>10</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="H7" s="2" t="s">
         <v>306</v>
@@ -2634,7 +2673,7 @@
         <v>306</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="K7" s="5">
         <v>0</v>
@@ -2669,7 +2708,7 @@
         <v>9</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="H8" s="2" t="s">
         <v>306</v>
@@ -2678,7 +2717,7 @@
         <v>306</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="K8" s="5">
         <v>0</v>
@@ -2713,7 +2752,7 @@
         <v>6</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="H9" s="2" t="s">
         <v>306</v>
@@ -2722,7 +2761,7 @@
         <v>306</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="K9" s="5">
         <v>0</v>
@@ -2757,7 +2796,7 @@
         <v>11</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="H10" s="2" t="s">
         <v>306</v>
@@ -2766,7 +2805,7 @@
         <v>306</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="K10" s="5">
         <v>0</v>
@@ -2801,7 +2840,7 @@
         <v>9</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="H11" s="2" t="s">
         <v>306</v>
@@ -2810,7 +2849,7 @@
         <v>306</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="K11" s="5">
         <v>0</v>
@@ -2845,7 +2884,7 @@
         <v>21</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="H12" s="2" t="s">
         <v>306</v>
@@ -2854,7 +2893,7 @@
         <v>306</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="K12" s="5">
         <v>0</v>
@@ -2889,7 +2928,7 @@
         <v>10</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="H13" s="2" t="s">
         <v>306</v>
@@ -2898,7 +2937,7 @@
         <v>306</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="K13" s="5">
         <v>0</v>
@@ -2933,7 +2972,7 @@
         <v>8</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="H14" s="2" t="s">
         <v>306</v>
@@ -2942,7 +2981,7 @@
         <v>306</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="K14" s="5">
         <v>0</v>
@@ -2977,7 +3016,7 @@
         <v>7</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="H15" s="2" t="s">
         <v>306</v>
@@ -2986,7 +3025,7 @@
         <v>306</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="K15" s="5">
         <v>0</v>
@@ -3021,7 +3060,7 @@
         <v>8</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="H16" s="2" t="s">
         <v>306</v>
@@ -3030,7 +3069,7 @@
         <v>306</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="K16" s="5">
         <v>0</v>
@@ -3065,7 +3104,7 @@
         <v>12</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="H17" s="2" t="s">
         <v>306</v>
@@ -3074,7 +3113,7 @@
         <v>306</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="K17" s="5">
         <v>0</v>
@@ -3109,7 +3148,7 @@
         <v>20</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="H18" s="2" t="s">
         <v>306</v>
@@ -3118,7 +3157,7 @@
         <v>306</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="K18" s="5">
         <v>0</v>
@@ -3147,13 +3186,13 @@
         <v>136</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="F19" s="5">
         <v>27</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="H19" s="2" t="s">
         <v>306</v>
@@ -3162,7 +3201,7 @@
         <v>306</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="K19" s="5">
         <v>0</v>
@@ -3191,13 +3230,13 @@
         <v>136</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="F20" s="5">
         <v>21</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="H20" s="2" t="s">
         <v>306</v>
@@ -3206,7 +3245,7 @@
         <v>306</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="K20" s="5">
         <v>0</v>
@@ -3235,13 +3274,13 @@
         <v>136</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="F21" s="5">
         <v>32</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="H21" s="2" t="s">
         <v>306</v>
@@ -3250,7 +3289,7 @@
         <v>306</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="K21" s="5">
         <v>0</v>
@@ -3285,7 +3324,7 @@
         <v>14</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="H22" s="2" t="s">
         <v>306</v>
@@ -3294,7 +3333,7 @@
         <v>306</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="K22" s="5">
         <v>0</v>
@@ -3329,7 +3368,7 @@
         <v>12</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="H23" s="2" t="s">
         <v>306</v>
@@ -3338,7 +3377,7 @@
         <v>306</v>
       </c>
       <c r="J23" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="K23" s="5">
         <v>0</v>
@@ -3373,7 +3412,7 @@
         <v>18</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="H24" s="2" t="s">
         <v>306</v>
@@ -3382,7 +3421,7 @@
         <v>306</v>
       </c>
       <c r="J24" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="K24" s="5">
         <v>0</v>
@@ -3417,7 +3456,7 @@
         <v>19</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="H25" s="2" t="s">
         <v>306</v>
@@ -3426,7 +3465,7 @@
         <v>306</v>
       </c>
       <c r="J25" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="K25" s="5">
         <v>0</v>
@@ -3461,7 +3500,7 @@
         <v>15</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="H26" s="2" t="s">
         <v>306</v>
@@ -3470,7 +3509,7 @@
         <v>306</v>
       </c>
       <c r="J26" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="K26" s="5">
         <v>0</v>
@@ -3505,7 +3544,7 @@
         <v>16</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="H27" s="2" t="s">
         <v>306</v>
@@ -3514,7 +3553,7 @@
         <v>306</v>
       </c>
       <c r="J27" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="K27" s="5">
         <v>0</v>
@@ -3549,7 +3588,7 @@
         <v>14</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="H28" s="2" t="s">
         <v>306</v>
@@ -3558,7 +3597,7 @@
         <v>306</v>
       </c>
       <c r="J28" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="K28" s="5">
         <v>0</v>
@@ -3593,7 +3632,7 @@
         <v>16</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="H29" s="2" t="s">
         <v>306</v>
@@ -3602,7 +3641,7 @@
         <v>306</v>
       </c>
       <c r="J29" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="K29" s="5">
         <v>0</v>
@@ -3637,7 +3676,7 @@
         <v>13</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="H30" s="2" t="s">
         <v>306</v>
@@ -3646,7 +3685,7 @@
         <v>306</v>
       </c>
       <c r="J30" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="K30" s="5">
         <v>0</v>
@@ -3681,7 +3720,7 @@
         <v>16</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="H31" s="2" t="s">
         <v>306</v>
@@ -3690,7 +3729,7 @@
         <v>306</v>
       </c>
       <c r="J31" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="K31" s="5">
         <v>0</v>
@@ -3725,7 +3764,7 @@
         <v>39</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="H32" s="2" t="s">
         <v>306</v>
@@ -3734,7 +3773,7 @@
         <v>306</v>
       </c>
       <c r="J32" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="K32" s="5">
         <v>0</v>
@@ -3769,7 +3808,7 @@
         <v>40</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="H33" s="2" t="s">
         <v>306</v>
@@ -3778,7 +3817,7 @@
         <v>306</v>
       </c>
       <c r="J33" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="K33" s="5">
         <v>0</v>
@@ -3813,7 +3852,7 @@
         <v>21</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="H34" s="2" t="s">
         <v>306</v>
@@ -3822,7 +3861,7 @@
         <v>306</v>
       </c>
       <c r="J34" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="K34" s="5">
         <v>0</v>
@@ -3857,7 +3896,7 @@
         <v>31</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="H35" s="2" t="s">
         <v>306</v>
@@ -3866,7 +3905,7 @@
         <v>306</v>
       </c>
       <c r="J35" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="K35" s="5">
         <v>0</v>
@@ -3901,7 +3940,7 @@
         <v>30</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="H36" s="2" t="s">
         <v>306</v>
@@ -3910,7 +3949,7 @@
         <v>306</v>
       </c>
       <c r="J36" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="K36" s="5">
         <v>0</v>
@@ -3945,7 +3984,7 @@
         <v>33</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="H37" s="2" t="s">
         <v>306</v>
@@ -3954,7 +3993,7 @@
         <v>306</v>
       </c>
       <c r="J37" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="K37" s="5">
         <v>0</v>
@@ -3989,7 +4028,7 @@
         <v>26</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="H38" s="2" t="s">
         <v>306</v>
@@ -3998,7 +4037,7 @@
         <v>306</v>
       </c>
       <c r="J38" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="K38" s="5">
         <v>0</v>
@@ -4033,7 +4072,7 @@
         <v>32</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="H39" s="2" t="s">
         <v>306</v>
@@ -4042,7 +4081,7 @@
         <v>306</v>
       </c>
       <c r="J39" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="K39" s="5">
         <v>0</v>
@@ -4077,7 +4116,7 @@
         <v>13</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="H40" s="2" t="s">
         <v>306</v>
@@ -4086,7 +4125,7 @@
         <v>306</v>
       </c>
       <c r="J40" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="K40" s="5">
         <v>0</v>
@@ -4121,7 +4160,7 @@
         <v>10</v>
       </c>
       <c r="G41" s="2" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="H41" s="2" t="s">
         <v>306</v>
@@ -4130,7 +4169,7 @@
         <v>306</v>
       </c>
       <c r="J41" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="K41" s="5">
         <v>0</v>
@@ -4165,7 +4204,7 @@
         <v>6</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="H42" s="2" t="s">
         <v>306</v>
@@ -4174,7 +4213,7 @@
         <v>306</v>
       </c>
       <c r="J42" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="K42" s="5">
         <v>0</v>
@@ -4209,7 +4248,7 @@
         <v>13</v>
       </c>
       <c r="G43" s="2" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="H43" s="2" t="s">
         <v>306</v>
@@ -4218,7 +4257,7 @@
         <v>306</v>
       </c>
       <c r="J43" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="K43" s="5">
         <v>0</v>
@@ -4253,7 +4292,7 @@
         <v>14</v>
       </c>
       <c r="G44" s="2" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="H44" s="2" t="s">
         <v>306</v>
@@ -4262,7 +4301,7 @@
         <v>306</v>
       </c>
       <c r="J44" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="K44" s="5">
         <v>0</v>
@@ -4285,215 +4324,347 @@
         <v>324</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="D45" s="2" t="s">
         <v>326</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="F45" s="5">
         <v>26</v>
       </c>
       <c r="G45" s="2" t="s">
+        <v>460</v>
+      </c>
+      <c r="H45" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="I45" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="J45" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="K45" s="5">
+        <v>0</v>
+      </c>
+      <c r="L45" s="5">
+        <v>0</v>
+      </c>
+      <c r="M45" s="5">
+        <v>0</v>
+      </c>
+      <c r="N45" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="116.25" customFormat="1" s="1">
+      <c r="A46" s="14" t="s">
         <v>461</v>
       </c>
-      <c r="H45" s="2" t="s">
-        <v>306</v>
-      </c>
-      <c r="I45" s="2" t="s">
-        <v>306</v>
-      </c>
-      <c r="J45" s="2" t="s">
-        <v>413</v>
-      </c>
-      <c r="K45" s="5">
-        <v>0</v>
-      </c>
-      <c r="L45" s="5">
-        <v>0</v>
-      </c>
-      <c r="M45" s="5">
-        <v>0</v>
-      </c>
-      <c r="N45" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="116.25" customFormat="1" s="1">
-      <c r="A46" s="15" t="s">
+      <c r="B46" s="14" t="s">
         <v>462</v>
       </c>
-      <c r="B46" s="15" t="s">
+      <c r="C46" s="14" t="s">
         <v>463</v>
       </c>
-      <c r="C46" s="15" t="s">
+      <c r="D46" s="14" t="s">
+        <v>326</v>
+      </c>
+      <c r="E46" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="F46" s="15">
+        <v>11</v>
+      </c>
+      <c r="G46" s="14" t="s">
         <v>464</v>
       </c>
-      <c r="D46" s="15" t="s">
+      <c r="H46" s="14" t="s">
+        <v>306</v>
+      </c>
+      <c r="I46" s="14" t="s">
+        <v>306</v>
+      </c>
+      <c r="J46" s="14" t="s">
+        <v>412</v>
+      </c>
+      <c r="K46" s="15">
+        <v>0</v>
+      </c>
+      <c r="L46" s="15">
+        <v>0</v>
+      </c>
+      <c r="M46" s="15">
+        <v>0</v>
+      </c>
+      <c r="N46" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="144" customFormat="1" s="1">
+      <c r="A47" s="14" t="s">
+        <v>465</v>
+      </c>
+      <c r="B47" s="14" t="s">
+        <v>466</v>
+      </c>
+      <c r="C47" s="14" t="s">
+        <v>467</v>
+      </c>
+      <c r="D47" s="14" t="s">
         <v>326</v>
       </c>
-      <c r="E46" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="F46" s="16">
-        <v>11</v>
-      </c>
-      <c r="G46" s="15" t="s">
-        <v>465</v>
-      </c>
-      <c r="H46" s="15" t="s">
-        <v>306</v>
-      </c>
-      <c r="I46" s="15" t="s">
-        <v>306</v>
-      </c>
-      <c r="J46" s="15" t="s">
-        <v>413</v>
-      </c>
-      <c r="K46" s="16">
-        <v>0</v>
-      </c>
-      <c r="L46" s="16">
-        <v>0</v>
-      </c>
-      <c r="M46" s="16">
-        <v>0</v>
-      </c>
-      <c r="N46" s="16">
-        <v>0</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="144" customFormat="1" s="1">
-      <c r="A47" s="15" t="s">
-        <v>466</v>
-      </c>
-      <c r="B47" s="15" t="s">
-        <v>467</v>
-      </c>
-      <c r="C47" s="15" t="s">
+      <c r="E47" s="14" t="s">
+        <v>160</v>
+      </c>
+      <c r="F47" s="15">
+        <v>14</v>
+      </c>
+      <c r="G47" s="14" t="s">
         <v>468</v>
       </c>
-      <c r="D47" s="15" t="s">
+      <c r="H47" s="14" t="s">
+        <v>306</v>
+      </c>
+      <c r="I47" s="14" t="s">
+        <v>306</v>
+      </c>
+      <c r="J47" s="14" t="s">
+        <v>412</v>
+      </c>
+      <c r="K47" s="15">
+        <v>0</v>
+      </c>
+      <c r="L47" s="15">
+        <v>0</v>
+      </c>
+      <c r="M47" s="15">
+        <v>0</v>
+      </c>
+      <c r="N47" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="151.5" customFormat="1" s="1">
+      <c r="A48" s="14" t="s">
+        <v>469</v>
+      </c>
+      <c r="B48" s="14" t="s">
+        <v>470</v>
+      </c>
+      <c r="C48" s="14" t="s">
+        <v>471</v>
+      </c>
+      <c r="D48" s="14" t="s">
+        <v>472</v>
+      </c>
+      <c r="E48" s="14" t="s">
+        <v>459</v>
+      </c>
+      <c r="F48" s="15">
+        <v>17</v>
+      </c>
+      <c r="G48" s="14" t="s">
+        <v>473</v>
+      </c>
+      <c r="H48" s="14" t="s">
+        <v>306</v>
+      </c>
+      <c r="I48" s="14" t="s">
+        <v>306</v>
+      </c>
+      <c r="J48" s="14" t="s">
+        <v>412</v>
+      </c>
+      <c r="K48" s="15">
+        <v>0</v>
+      </c>
+      <c r="L48" s="15">
+        <v>0</v>
+      </c>
+      <c r="M48" s="15">
+        <v>0</v>
+      </c>
+      <c r="N48" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="19.5">
+      <c r="A49" s="16" t="s">
+        <v>474</v>
+      </c>
+      <c r="B49" s="16" t="s">
+        <v>475</v>
+      </c>
+      <c r="C49" s="16" t="s">
+        <v>476</v>
+      </c>
+      <c r="D49" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="E49" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="F49" s="17">
+        <v>19</v>
+      </c>
+      <c r="G49" s="16" t="s">
+        <v>477</v>
+      </c>
+      <c r="H49" s="16" t="s">
+        <v>306</v>
+      </c>
+      <c r="I49" s="16" t="s">
+        <v>306</v>
+      </c>
+      <c r="J49" s="16" t="s">
+        <v>412</v>
+      </c>
+      <c r="K49" s="17">
+        <v>0</v>
+      </c>
+      <c r="L49" s="17">
+        <v>0</v>
+      </c>
+      <c r="M49" s="17">
+        <v>0</v>
+      </c>
+      <c r="N49" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="50" customHeight="1" ht="19.5">
+      <c r="A50" s="16" t="s">
+        <v>478</v>
+      </c>
+      <c r="B50" s="16" t="s">
+        <v>479</v>
+      </c>
+      <c r="C50" s="16" t="s">
+        <v>480</v>
+      </c>
+      <c r="D50" s="16" t="s">
+        <v>481</v>
+      </c>
+      <c r="E50" s="16" t="s">
+        <v>160</v>
+      </c>
+      <c r="F50" s="17">
+        <v>10</v>
+      </c>
+      <c r="G50" s="16" t="s">
+        <v>482</v>
+      </c>
+      <c r="H50" s="16" t="s">
+        <v>306</v>
+      </c>
+      <c r="I50" s="16" t="s">
+        <v>306</v>
+      </c>
+      <c r="J50" s="16" t="s">
+        <v>412</v>
+      </c>
+      <c r="K50" s="17">
+        <v>0</v>
+      </c>
+      <c r="L50" s="17">
+        <v>0</v>
+      </c>
+      <c r="M50" s="17">
+        <v>0</v>
+      </c>
+      <c r="N50" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="51" customHeight="1" ht="19.5">
+      <c r="A51" s="16" t="s">
+        <v>483</v>
+      </c>
+      <c r="B51" s="16" t="s">
+        <v>484</v>
+      </c>
+      <c r="C51" s="16" t="s">
+        <v>485</v>
+      </c>
+      <c r="D51" s="16" t="s">
+        <v>231</v>
+      </c>
+      <c r="E51" s="16" t="s">
+        <v>232</v>
+      </c>
+      <c r="F51" s="17">
+        <v>34</v>
+      </c>
+      <c r="G51" s="16" t="s">
+        <v>486</v>
+      </c>
+      <c r="H51" s="16" t="s">
+        <v>306</v>
+      </c>
+      <c r="I51" s="16" t="s">
+        <v>306</v>
+      </c>
+      <c r="J51" s="16" t="s">
+        <v>412</v>
+      </c>
+      <c r="K51" s="17">
+        <v>0</v>
+      </c>
+      <c r="L51" s="17">
+        <v>0</v>
+      </c>
+      <c r="M51" s="17">
+        <v>0</v>
+      </c>
+      <c r="N51" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="52" customHeight="1" ht="402" customFormat="1" s="1">
+      <c r="A52" s="4" t="s">
+        <v>332</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>487</v>
+      </c>
+      <c r="D52" s="2" t="s">
         <v>326</v>
       </c>
-      <c r="E47" s="15" t="s">
-        <v>160</v>
-      </c>
-      <c r="F47" s="16">
-        <v>14</v>
-      </c>
-      <c r="G47" s="15" t="s">
-        <v>469</v>
-      </c>
-      <c r="H47" s="15" t="s">
-        <v>306</v>
-      </c>
-      <c r="I47" s="15" t="s">
-        <v>306</v>
-      </c>
-      <c r="J47" s="15" t="s">
-        <v>413</v>
-      </c>
-      <c r="K47" s="16">
-        <v>0</v>
-      </c>
-      <c r="L47" s="16">
-        <v>0</v>
-      </c>
-      <c r="M47" s="16">
-        <v>0</v>
-      </c>
-      <c r="N47" s="16">
-        <v>0</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="151.5" customFormat="1" s="1">
-      <c r="A48" s="15" t="s">
-        <v>470</v>
-      </c>
-      <c r="B48" s="15" t="s">
-        <v>471</v>
-      </c>
-      <c r="C48" s="15" t="s">
-        <v>472</v>
-      </c>
-      <c r="D48" s="15" t="s">
-        <v>473</v>
-      </c>
-      <c r="E48" s="15" t="s">
-        <v>460</v>
-      </c>
-      <c r="F48" s="16">
-        <v>17</v>
-      </c>
-      <c r="G48" s="15" t="s">
-        <v>474</v>
-      </c>
-      <c r="H48" s="15" t="s">
-        <v>306</v>
-      </c>
-      <c r="I48" s="15" t="s">
-        <v>306</v>
-      </c>
-      <c r="J48" s="15" t="s">
-        <v>413</v>
-      </c>
-      <c r="K48" s="16">
-        <v>0</v>
-      </c>
-      <c r="L48" s="16">
-        <v>0</v>
-      </c>
-      <c r="M48" s="16">
-        <v>0</v>
-      </c>
-      <c r="N48" s="16">
-        <v>0</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="402" customFormat="1" s="1">
-      <c r="A49" s="4" t="s">
-        <v>332</v>
-      </c>
-      <c r="B49" s="2" t="s">
-        <v>333</v>
-      </c>
-      <c r="C49" s="2" t="s">
-        <v>475</v>
-      </c>
-      <c r="D49" s="2" t="s">
-        <v>326</v>
-      </c>
-      <c r="E49" s="2" t="s">
-        <v>460</v>
-      </c>
-      <c r="F49" s="5">
+      <c r="E52" s="2" t="s">
+        <v>459</v>
+      </c>
+      <c r="F52" s="5">
         <v>43</v>
       </c>
-      <c r="G49" s="2" t="s">
-        <v>476</v>
-      </c>
-      <c r="H49" s="2" t="s">
-        <v>306</v>
-      </c>
-      <c r="I49" s="2" t="s">
-        <v>306</v>
-      </c>
-      <c r="J49" s="2" t="s">
-        <v>413</v>
-      </c>
-      <c r="K49" s="5">
-        <v>0</v>
-      </c>
-      <c r="L49" s="5">
-        <v>0</v>
-      </c>
-      <c r="M49" s="5">
-        <v>0</v>
-      </c>
-      <c r="N49" s="5">
+      <c r="G52" s="2" t="s">
+        <v>488</v>
+      </c>
+      <c r="H52" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="I52" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="J52" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="K52" s="5">
+        <v>0</v>
+      </c>
+      <c r="L52" s="5">
+        <v>0</v>
+      </c>
+      <c r="M52" s="5">
+        <v>0</v>
+      </c>
+      <c r="N52" s="5">
         <v>0</v>
       </c>
     </row>
@@ -4509,14 +4680,14 @@
   </sheetPr>
   <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="13" width="14.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="14" width="15.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="13" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="13" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="12" width="14.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="13" width="15.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="12" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="12" width="14.147857142857141" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
@@ -4697,90 +4868,80 @@
       <c r="C13" s="8" t="s">
         <v>389</v>
       </c>
-      <c r="D13" s="11" t="s">
-        <v>390</v>
-      </c>
+      <c r="D13" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
       <c r="A14" s="10" t="s">
+        <v>390</v>
+      </c>
+      <c r="B14" s="8" t="s">
         <v>391</v>
       </c>
-      <c r="B14" s="8" t="s">
-        <v>392</v>
-      </c>
       <c r="C14" s="8"/>
-      <c r="D14" s="11" t="s">
-        <v>390</v>
-      </c>
+      <c r="D14" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
       <c r="A15" s="10" t="s">
+        <v>392</v>
+      </c>
+      <c r="B15" s="8" t="s">
         <v>393</v>
       </c>
-      <c r="B15" s="8" t="s">
-        <v>394</v>
-      </c>
       <c r="C15" s="8"/>
-      <c r="D15" s="11" t="s">
-        <v>390</v>
-      </c>
+      <c r="D15" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
       <c r="A16" s="10" t="s">
+        <v>394</v>
+      </c>
+      <c r="B16" s="8" t="s">
         <v>395</v>
-      </c>
-      <c r="B16" s="8" t="s">
-        <v>396</v>
       </c>
       <c r="C16" s="8"/>
       <c r="D16" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
       <c r="A17" s="8" t="s">
+        <v>396</v>
+      </c>
+      <c r="B17" s="8" t="s">
         <v>397</v>
-      </c>
-      <c r="B17" s="8" t="s">
-        <v>398</v>
       </c>
       <c r="C17" s="10"/>
       <c r="D17" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
-      <c r="A18" s="11" t="s">
-        <v>390</v>
-      </c>
+      <c r="A18" s="8"/>
       <c r="B18" s="8" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="C18" s="10"/>
       <c r="D18" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5">
       <c r="A19" s="8" t="s">
+        <v>399</v>
+      </c>
+      <c r="B19" s="8" t="s">
         <v>400</v>
-      </c>
-      <c r="B19" s="8" t="s">
-        <v>401</v>
       </c>
       <c r="C19" s="10"/>
       <c r="D19" s="10"/>
     </row>
     <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5">
       <c r="A20" s="8" t="s">
+        <v>401</v>
+      </c>
+      <c r="B20" s="8" t="s">
         <v>402</v>
-      </c>
-      <c r="B20" s="8" t="s">
-        <v>403</v>
       </c>
       <c r="C20" s="10"/>
       <c r="D20" s="10"/>
     </row>
     <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="19.5">
-      <c r="A21" s="11" t="s">
-        <v>390</v>
-      </c>
+      <c r="A21" s="8"/>
       <c r="B21" s="8" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="C21" s="10"/>
       <c r="D21" s="10"/>
@@ -4788,7 +4949,7 @@
     <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="19.5">
       <c r="A22" s="8"/>
       <c r="B22" s="8" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="C22" s="10"/>
       <c r="D22" s="10"/>
@@ -4809,7 +4970,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="19.5">
       <c r="A25" s="10"/>
-      <c r="B25" s="12"/>
+      <c r="B25" s="11"/>
       <c r="C25" s="10"/>
       <c r="D25" s="10"/>
     </row>

</xml_diff>